<commit_message>
updated refresh jobs code
</commit_message>
<xml_diff>
--- a/internships.xlsx
+++ b/internships.xlsx
@@ -483,12 +483,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Business Development (Sales) - Web3</t>
+          <t>Admission Counsellor (Female)</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>About the work from home job/internship    Selected intern's day-to-day responsibilities include: 1. Research and identify potential institutional investors (family offices, fund managers)2. Create personalized outreach campaigns for different investor segments3. Manage investor communications and follow-up sequences4. Support partnership development with Web3 communities5. Assist in preparing investment materials and presentations6. Track and report on BD metrics and pipeline progressSkill(s) requiredBlockchainClient Relationship Management (CRM)CryptographyEnglish Proficiency (Spoken)English Proficiency (Written)Financial literacyLead GenerationResearch and AnalyticsSales StrategyEarn certifications in these skillsLearn BlockchainLearn Business CommunicationLearn Stocks and TradingLearn HyperledgerLearn Research and AnalyticsWho can applyOnly those candidates can apply who:                1. are available for the work from home job/internship                                    2. can start the work from home job/internship between 12th Jul'25 and 16th Aug'25                                    3. are available for duration of 4 months                                    4. have relevant skills and interests                    * Women wanting to start/restart their career can also apply.Other requirements                    1. Students pursuing BBA/MBA/economics/finance                                    2. Web3/Crypto knoweldege required                                    3. Freshers with strong analytical skills                                    4. Excellent written English (mandatory)                                    5. Available 3-4 hours daily                                    6. Own laptop &amp; Internet required                PerksCertificate Letter of recommendation Flexible work hoursAdditional informationStipend Structure:Fixed pay: ₹ 5,000 - 15,000 /month                    Incentive pay: ₹ 8,000 /month                     Number of openings        4                        About Podha Protocol                        Podha Protocol is a web3 yield generation platform via real real-world digital asset management company. Recognized as a top-tier digital asset yield platform, Podha delivers reliable and forward-thinking yield solutions that bolster the digital asset economy.    Activity on InternshalaHiring since May 202515 opportunities posted                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
+          <t>About the internship    We are hiring a telecaller intern (female candidate) who can join immediately.Selected intern's day-to-day responsibilities include:1. Interact with students telephonically &amp; convert leads into admissions. 2. Offer MBBS abroad admission services to the students/parents 3. Set appointments for students for office visits or Zoom meetings.Skill(s) requiredEffective CommunicationSalesEarn certifications in these skillsLearn Business CommunicationLearn Digital MarketingLearn Business AnalyticsWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 5th Jul'25 and 9th Aug'25                                    3. are available for duration of 2 months                                    4. are from Pune only                                    5. have relevant skills and interests                    * Women wanting to start/restart their career can also apply.Other requirements                    1. Should have a passion to grow &amp; progress in life.                                    2. Aggressive in approach.                                    3. Good communication in Marathi must.                PerksCertificate Letter of recommendation Informal dress codeAdditional informationStipend Structure:Fixed pay: ₹ 7,000 - 10,000 /month                    Incentive pay: ₹ 200 - 1,000 /month                     Number of openings        2                        About Bright EduWorld                Website         We are a medical e-learning company mentoring medical students &amp; optimizing their abilities, approach, and mindset.    Activity on InternshalaHiring since September 20238 opportunities posted1 candidate hired                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -506,24 +506,24 @@
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:10</t>
+          <t>2025-07-20 10:40:52</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/work-from-home-business-development-sales-web3-internship-at-podha-protocol1752338121</t>
+          <t>https://internshala.com/internship/detail/telecaller-female-internship-in-pune-at-bright-eduworld1751749920</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Virtual Charity Drive</t>
+          <t>Human Resource</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>About the work from home job/internship    Join our 'Virtual Charity Drive Internship' and become a driving force behind our mission to make a difference. As an intern, you'll focus on fundraising through innovative virtual campaigns aimed at supporting various charitable causes. Selected intern's day-to-day responsibilities include devising and implementing strategies to engage donors online, and leveraging social media platforms and digital tools. This internship provides a unique opportunity to gain practical experience in fundraising, digital marketing, and project management while making a meaningful impact on communities in need.Skill(s) requiredEffective CommunicationEarn certifications in these skillsLearn Creative WritingLearn Business CommunicationLearn Digital MarketingLearn Business AnalyticsWho can applyOnly those candidates can apply who:                1. are available for the work from home job/internship                                    2. can start the work from home job/internship between 18th Jul'25 and 22nd Aug'25                                    3. are available for duration of 1 month                                    4. have relevant skills and interests                    * Women wanting to start/restart their career can also apply.PerksCertificate Letter of recommendationNumber of openings        500                        About Basti Ki Pathshala Foundation                        Basti Ki Pathshala Foundation is a Government-registered organization established under the Indian Societies Act of 1860. We are a grassroots organization dedicated to breaking the barriers of education in underserved communities. Founded with a mission to provide quality education to children living in slum areas, we strive to create a nurturing learning environment where every child has the opportunity to thrive. Through innovative teaching methods, community engagement, and partnerships, we empower children with the knowledge and skills they need to build a brighter future. Our commitment extends beyond the classroom as we work towards bridging the educational gap and fostering long-term sustainable change in the lives of marginalized families.    Activity on InternshalaHiring since February 20241083 opportunities posted14496 candidates hired                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
+          <t>About the internship    Selected interns day-to-day responsibilities:1. Conducting sourcing activities for open positions2. Involving in recruitment and selection processes (resume screening, screening calls, interviews, etc.)3. Making SOPs and policies4. Conducting onboarding and exit process5. Handling payroll using HRIS software6. Handling other HR-related jobs assigned from time to timeSkill(s) requiredEnglish Proficiency (Spoken)English Proficiency (Written)MS-ExcelMS-WordOperationsRecruitmentEarn certifications in these skillsLearn Business CommunicationLearn MS-ExcelLearn about RecruitmentWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 8th Jul'25 and 12th Aug'25                                    3. are available for duration of 4 months                                    4. are from Gandhinagar only                                    5. have relevant skills and interests                    PerksLetter of recommendation Flexible work hours 5 days a weekNumber of openings        1                        About Get Structured Consulting Services OPC Private Limited                Website         We are a one-stop solution for all the HR needs of new-age startups. At GetStructured, our mission is to empower businesses to achieve their full potential by providing expert human resources support and guidance. We believe that a strong HR function is essential to the success of any organization, and we are dedicated to helping our clients build and maintain a high-performing, engaged, and effective workforce.    Activity on InternshalaHiring since June 202322 opportunities posted1 candidate hired                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -541,24 +541,24 @@
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:11</t>
+          <t>2025-07-20 10:40:53</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/work-from-home-part-time-virtual-charity-drive-internship-at-basti-ki-pathshala-foundation1752833362</t>
+          <t>https://internshala.com/internship/detail/human-resource-internship-in-gandhinagar-at-get-structured-consulting-services-opc-private-limited1751975462</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Human Resource</t>
+          <t>Videography</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>About the internship    Selected interns day-to-day responsibilities:1. Conducting sourcing activities for open positions2. Involving in recruitment and selection processes (resume screening, screening calls, interviews, etc.)3. Making SOPs and policies4. Conducting onboarding and exit process5. Handling payroll using HRIS software6. Handling other HR-related jobs assigned from time to timeSkill(s) requiredEnglish Proficiency (Spoken)English Proficiency (Written)MS-ExcelMS-WordOperationsRecruitmentEarn certifications in these skillsLearn Business CommunicationLearn MS-ExcelLearn about RecruitmentWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 8th Jul'25 and 12th Aug'25                                    3. are available for duration of 4 months                                    4. are from Gandhinagar only                                    5. have relevant skills and interests                    PerksLetter of recommendation Flexible work hours 5 days a weekNumber of openings        1                        About Get Structured Consulting Services OPC Private Limited                Website         We are a one-stop solution for all the HR needs of new-age startups. At GetStructured, our mission is to empower businesses to achieve their full potential by providing expert human resources support and guidance. We believe that a strong HR function is essential to the success of any organization, and we are dedicated to helping our clients build and maintain a high-performing, engaged, and effective workforce.    Activity on InternshalaHiring since June 202322 opportunities posted1 candidate hired                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
+          <t>About the internship    As a Videography at The Trading Fox, you will have the exciting opportunity to showcase your skills in video making, videography, and photography. You will work closely with our team to create captivating visual content for our brand. 1.  Capture high-quality video footage for promotional videos and social media content.2. Enhance video content to ensure a polished final product.3. Help set up and operate equipment for video shoots, including cameras, lighting, and audio.4. Manage and organize video files and footage to maintain a streamlined workflow.5. Stay up-to-date on industry trends and best practices to bring fresh ideas to our projects.Join us at The Trading Fox and help us bring our brand to life through the power of video.Skill(s) requiredPhotographyVideographyVideo MakingEarn certifications in these skillsLearn Adobe Premiere ProLearn PhotographyLearn Video EditingWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 17th Jul'25 and 21st Aug'25                                    3. are available for duration of 2 months                                    4. are from Jaipur only                                    5. have relevant skills and interests                    PerksCertificate Letter of recommendation Informal dress codeNumber of openings        2                        About The Trading Fox                        Trading Fox PVT. LTD. is a premier trading and finance firm dedicated to empowering clients through strategic investment solutions and expert financial guidance. We specialize in a wide range of services, including equities, commodities, forex, and derivatives trading, tailored to meet the diverse needs of individual investors and institutional clients alike.Our team of seasoned professionals leverages advanced analytics and market insights to identify lucrative opportunities and mitigate risks. We pride ourselves on our commitment to transparency, integrity, and personalized service, ensuring that our clients are well-informed and equipped to make confident financial decisions.At Trading Fox, we strive to foster long-term relationships built on trust and performance, helping our clients navigate the complexities of the financial markets to achieve their financial goals.    Activity on InternshalaHiring since October 2024108 opportunities posted                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -576,24 +576,24 @@
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:12</t>
+          <t>2025-07-20 10:40:54</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/human-resource-internship-in-gandhinagar-at-get-structured-consulting-services-opc-private-limited1751975462</t>
+          <t>https://internshala.com/internship/detail/videography-internship-in-jaipur-at-the-trading-fox1752734340</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Operation &amp; Maintenance Supervisor</t>
+          <t>Field Sales</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>About the internship    We're looking for a hands-on male intern from a Civil or Electrical Engineering background to support daily operations and maintenance at a sewage treatment plant (STP) site. Perfect for those who want practical infrastructure experience in real field conditions.Selected intern's day-to-day responsibilities include:1. Assist in the daily maintenance of the STP plant2. Record and monitor key operational parameters (flow rates, pressure, etc.)3. Support in resolving electrical/control panel issues4. Help manage sludge removal, aeration processes, and chemical dosing5. Maintain logbooks, checklists, and operational records6. Coordinate with site engineers for routine checks and reporting7. Assist in spare part tracking and minor repair coordination8. Learn and follow safety and compliance protocols9. Join daily review or vendor meetings where needed10. Share basic reports or updates with supervisorsWho Should Apply:1. Final-year students or fresh graduates in civil or electrical engineering2. Must be willing to stay full-time on-site during the internship3. Interested in utilities, infrastructure, or sustainable project work4. Ready to learn in a real, high-responsibility environment5. Comfortable with routine tasks and hands-on workWhat You'll Gain:1. On-ground experience at a live STP infrastructure project2. Exposure to real-time engineering practices and team coordination3. Mentorship from professionals in the infra/utilities domain4. Certificate + Letter of Recommendation based on performance5. Possibility of a Pre-Placement Offer (PPO) for outstanding interns6. Improved resume and technical confidencePlease only apply if you are available for a minimum 6-month full-time on-site internship.Skill(s) requiredEngineering DrawingEngineering SurveyingTechnical AnalysisEarn certifications in these skillsLearn AutoCADLearn STAAD ProLearn RevitLearn AutoCAD 3DLearn Engineering DrawingWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 18th Jun'25 and 23rd Jul'25                                    3. are available for duration of 6 months                                    4. have relevant skills and interests                    Other requirements                    1. Students from other engineering backgrounds with a strong interest in infrastructure/utilities may also apply, but only if they are available for a minimum 6-month full-time on-site internship.                Number of openings        2                        About Movi Ecoserve Private Limited                        Movi Ecoserve works in sustainable technologies. We work majorly with the government and municipalities in pan India.     Activity on InternshalaHiring since February 202261 opportunities posted3 candidates hired                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
+          <t>About the internship    As a field &amp; sales marketing intern, you'll work closely with the marketing and operations team to promote the mission and products through grassroots outreach, retail engagement, and local campaign activities. This role is ideal for students passionate about sustainability, marketing, and rural development.Selected intern's day-to-day responsibilities include: 1. Assist in field sales drives, including product demos at local shops, events, or stalls2. Help execute local marketing campaigns (flyers, WhatsApp promotions, on-ground surveys)3. Support the onboarding of local retailers, organic stores, and individual customers4. Engage with customers and collect feedback on products like A2 milk, ghee, and soaps5. Represent the brand at community events, farmers' markets, or exhibitions6. Maintain daily records of outreach, leads, and customer interactions7. Coordinate with internal teams for delivery, packaging, and logistics trackingIdeal candidate:1. Education: pursuing/recently completed a degree in marketing, agriculture, rural management, or social work2. Skills: strong communication (Marathi/Hindi preferred), people skills, and willingness to travel locally3. Passionate about sustainability, animal welfare, and social impact4. Self-driven, eager to learn, and comfortable with on-ground activitiesWhat you'll learn:1. Grassroots marketing strategy and execution2. Sales techniques and customer engagement in real-world settings3. Insight into rural livelihood, sustainable agriculture, and indigenous dairy practices4. Exposure to a mission-driven start-up environment with real social impactSkill(s) requiredEffective CommunicationEmail MarketingEnglish Proficiency (Spoken)Hindi Proficiency (Spoken)Interpersonal skillsMS-OfficeEarn certifications in these skillsLearn Email MarketingLearn Business CommunicationLearn MS-ExcelWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 2nd Jul'25 and 6th Aug'25                                    3. are available for duration of 4 months                                    4. are from Pune only                                    5. have relevant skills and interests                    PerksCertificate Letter of recommendationAdditional informationStipend Structure:Fixed pay: ₹ 10,000 - 12,000 /month                    Incentive pay: ₹ 2,000 /month                     Number of openings        5                        About SOLARTS                        We are into health awareness and consultancy on disease control and cures. We offer one of the best organic health products in India and our company is a pure organic ayurvedic medicine based company.    Activity on InternshalaHiring since October 20182 opportunities posted                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -611,24 +611,24 @@
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:13</t>
+          <t>2025-07-20 10:40:55</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/operation-maintenance-supervisor-internship-in-mumbai-at-movi-ecoserve-private-limited1750307830</t>
+          <t>https://internshala.com/internship/detail/field-sales-internship-in-pune-at-solarts1751444830</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Architecture</t>
+          <t>Video Animator</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>About the internship    THD Design Studio is seeking an Architecture Intern who is proficient in AutoCAD, Adobe Photoshop, Google SketchUp, Autodesk 3ds Max, and MS-Office to join our team. As an intern, you will have the opportunity to work on a variety of projects and grow your skills in a collaborative and creative environment.1. Assist with drafting and designing architectural plans using AutoCAD.2. Create visually stunning presentations and renderings using Adobe Photoshop.3. Develop 3D models and animations with Google SketchUp and Autodesk 3ds Max.4. Collaborate with team members to brainstorm and problem solve design challenges.5. Conduct research on industry trends and best practices to incorporate into projects.6. Attend client meetings and presentations to contribute ideas and insights.7. Support the team with administrative tasks and project management duties as needed.If you are a motivated and talented individual with a passion for architecture and design, we want to hear from you! Join us at THD Design Studio and take the first step towards a successful career in the industry. Apply now and showcase your skills in a professional setting.Skill(s) requiredAdobe PhotoshopAutoCADAutodesk 3ds MaxGoogle SketchUp MS-OfficeEarn certifications in these skillsLearn Adobe PhotoshopLearn AutoCADLearn MS-ExcelWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 9th Jul'25 and 13th Aug'25                                    3. are available for duration of 4 months                                    4. are from Thane, Navi Mumbai, Mumbai only                                    5. have relevant skills and interests                    PerksCertificate Letter of recommendation Informal dress codeNumber of openings        2                        About HD Design Studio                Instagram page         HD Design Studio is a Mumbai-based firm of experienced professionals offering comprehensive services in architecture, interior design, and urban design to residential, commercial, and institutional clients. In addition to extensive experience in all the architectural processes from designing to construction and execution, HDDS is actively involved in providing clients with the following services: architecture, interior design, residential design, historic renovations, site analysis, and feasibility, zoning and code consulting, building department expediting, municipal department approvals, dot approvals, landmark approvals, condominium subdivisions, and tenant reviews.    Activity on InternshalaHiring since November 202110 opportunities posted                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
+          <t>About the internship    Selected intern's day-to-day responsibilities include: 1. Bring creative vision to life: Use storytelling skills to create engaging animations2. Master animation tools: Work with Adobe After Effects, Premiere Pro, Illustrator, Photoshop, or equivalent software3. Ensure high-quality output: Deliver polished and detail-oriented animations4. Collaborate effectively: Communicate well with cross-functional teams to align on project goalsSkill(s) requiredAdobe After EffectsAdobe AnimateAdobe Creative SuiteAdobe IllustratorAdobe PhotoshopFigmaEarn certifications in these skillsLearn Adobe After EffectsLearn Colour Theory for DesignersLearn Adobe PhotoshopLearn Adobe Premiere ProLearn FigmaWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 5th Jul'25 and 9th Aug'25                                    3. are available for duration of 3 months                                    4. are from Jaipur only                                    5. have relevant skills and interests                    Other requirements                    1. Educational background: Currently enrolled in or recently graduated from animation, visual arts, multimedia design, or related programs                                    2. Technical knowledge: A basic understanding of video editing tools and techniques is preferred                                    3. Portfolio: Samples of previous animation work (optional but recommended)                                    4. Experience: Prior experience in related fields is a plus                PerksCertificateNumber of openings        1                        About Travel Lykke Private Limited                Website         We are a travel brand curating unique, experiential &amp; sustainable holidays for you. Our trips are not limited to usual travel arrangements. We design unique, immersive experiences that make their mark in your heart. We also believe in sustainable tourism. We try to make our trips as environmentally friendly as possible and engage local communities in the destinations. Other than the usual blah blah blah, we are a bunch of youngsters, insanely passionate about travel. We think of you as our future friends and not just customers.    Activity on InternshalaHiring since February 202527 opportunities posted13 candidates hired                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -646,24 +646,24 @@
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:13</t>
+          <t>2025-07-20 10:40:55</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/architecture-internship-in-multiple-locations-at-hd-design-studio1752057921</t>
+          <t>https://internshala.com/internship/detail/video-animator-internship-in-jaipur-at-travel-lykke-private-limited1751707788</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Admission Counsellor (Female)</t>
+          <t>Architecture</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>About the internship    We are hiring a telecaller intern (female candidate) who can join immediately.Selected intern's day-to-day responsibilities include:1. Interact with students telephonically &amp; convert leads into admissions. 2. Offer MBBS abroad admission services to the students/parents 3. Set appointments for students for office visits or Zoom meetings.Skill(s) requiredEffective CommunicationSalesEarn certifications in these skillsLearn Business CommunicationLearn Digital MarketingLearn Business AnalyticsWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 5th Jul'25 and 9th Aug'25                                    3. are available for duration of 2 months                                    4. are from Pune only                                    5. have relevant skills and interests                    * Women wanting to start/restart their career can also apply.Other requirements                    1. Should have a passion to grow &amp; progress in life.                                    2. Aggressive in approach.                                    3. Good communication in Marathi must.                PerksCertificate Letter of recommendation Informal dress codeAdditional informationStipend Structure:Fixed pay: ₹ 7,000 - 10,000 /month                    Incentive pay: ₹ 200 - 1,000 /month                     Number of openings        2                        About Bright EduWorld                Website         We are a medical e-learning company mentoring medical students &amp; optimizing their abilities, approach, and mindset.    Activity on InternshalaHiring since September 20238 opportunities posted1 candidate hired                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
+          <t>About the internship    THD Design Studio is seeking an Architecture Intern who is proficient in AutoCAD, Adobe Photoshop, Google SketchUp, Autodesk 3ds Max, and MS-Office to join our team. As an intern, you will have the opportunity to work on a variety of projects and grow your skills in a collaborative and creative environment.1. Assist with drafting and designing architectural plans using AutoCAD.2. Create visually stunning presentations and renderings using Adobe Photoshop.3. Develop 3D models and animations with Google SketchUp and Autodesk 3ds Max.4. Collaborate with team members to brainstorm and problem solve design challenges.5. Conduct research on industry trends and best practices to incorporate into projects.6. Attend client meetings and presentations to contribute ideas and insights.7. Support the team with administrative tasks and project management duties as needed.If you are a motivated and talented individual with a passion for architecture and design, we want to hear from you! Join us at THD Design Studio and take the first step towards a successful career in the industry. Apply now and showcase your skills in a professional setting.Skill(s) requiredAdobe PhotoshopAutoCADAutodesk 3ds MaxGoogle SketchUp MS-OfficeEarn certifications in these skillsLearn Adobe PhotoshopLearn AutoCADLearn MS-ExcelWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 9th Jul'25 and 13th Aug'25                                    3. are available for duration of 4 months                                    4. are from Thane, Navi Mumbai, Mumbai only                                    5. have relevant skills and interests                    PerksCertificate Letter of recommendation Informal dress codeNumber of openings        2                        About HD Design Studio                Instagram page         HD Design Studio is a Mumbai-based firm of experienced professionals offering comprehensive services in architecture, interior design, and urban design to residential, commercial, and institutional clients. In addition to extensive experience in all the architectural processes from designing to construction and execution, HDDS is actively involved in providing clients with the following services: architecture, interior design, residential design, historic renovations, site analysis, and feasibility, zoning and code consulting, building department expediting, municipal department approvals, dot approvals, landmark approvals, condominium subdivisions, and tenant reviews.    Activity on InternshalaHiring since November 202110 opportunities posted                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -681,24 +681,24 @@
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:14</t>
+          <t>2025-07-20 10:40:56</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/telecaller-female-internship-in-pune-at-bright-eduworld1751749920</t>
+          <t>https://internshala.com/internship/detail/architecture-internship-in-multiple-locations-at-hd-design-studio1752057921</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Design &amp; Communication</t>
+          <t>Market Research</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>About the internship    Selected intern's day-to-day responsibilities include: A. Graphic design &amp; visual content:1. Create visuals for social media, newsletters, website banners, presentations, pitch decks, etc.2. Design campaign assets like posters, digital ads, stories, GIFs, thumbnails, and email headers3. Maintain brand consistency across all designs (colors, fonts, layout, tone)4. Collaborate with marketing and content teams to turn ideas into engaging visualsB. Brand communication &amp; messaging:1. Assist in writing clear, compelling copy for campaigns, captions, brochures, etc.2. Help refine tone of voice across platforms to align with brand identity3. Support storytelling across platforms (visual + written) for product, brand, or founder narrativeC. Asset management:1. Organize and maintain brand asset folders (logos, fonts, templates, content banks)2. Keep a repository of past work for easy access and performance review3. Update and manage brand guideline documents if neededD. Campaign &amp; creative strategy support:1. Help brainstorm for creative campaigns, product launches, or seasonal content2. Assist in preparing mood boards, mockups, or presentation decks for internal reviews or clients3. Research industry trends and competitor content for design and tone benchmarksE. Content production assistance:1. Support photoshoots or video shoots (creative direction, layout, styling help)2. Edit short video snippets or story-based content using basic tools (optional but useful)3. Coordinate with freelancers or vendors (printers, photographers, editors)F. Cross-team collaboration:1. Work closely with the social media, marketing, and product teams2. Assist in internal communication design (event invites, internal notices, presentations)3. Support event branding and communication materials (digital invites, posters, handouts)Skill(s) requiredCanvaMS-PowerPointEarn certifications in these skillsLearn Graphic DesignLearn Creative WritingLearn Digital MarketingLearn Business AnalyticsWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 2nd Jul'25 and 6th Aug'25                                    3. are available for duration of 6 months                                    4. have relevant skills and interests                    Other requirements                    1. Should know Canva Powerpoint and interest in emerging tech/ media is a plus.                PerksCertificate Letter of recommendationNumber of openings        2                        About Movi Ecoserve Private Limited                        Movi Ecoserve works in sustainable technologies. We work majorly with the government and municipalities in pan India.     Activity on InternshalaHiring since February 202261 opportunities posted3 candidates hired                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
+          <t>About the internship    Are you passionate about market research? Do you have strong communication skills? Join our Startup - Lohagarh Software Solutions Private Limited as a Market Research intern and gain hands-on experience in the world of education &amp; counselling business &amp; technology Selected intern's day-to-day responsibilities include:1. Conduct market research to identify Education, Counselling &amp; Career trends and opportunities in the industry.2. Create a list of Schools, Tuition centres, etc and make Field Visits to collect additional data and validate the Startup Hypothesis.3. Analyze data using MS-Excel to generate insights and recommendations.4. Assist in creating reports and presentations for internal and external stakeholders.5. Collaborate with founders in refining and executing their business idea. 6. Support the team in developing strategies and marketing campaigns.This is a fantastic opportunity for someone looking to kickstart their career in market research and make a real impact in a fast-paced and dynamic environment. Apply now and take the first step towards a rewarding career with us!Skill(s) requiredEffective CommunicationInterpersonal skillsMS-OfficePresentation skillsResearch and AnalyticsSelf-learningEarn certifications in these skillsLearn MS-ExcelLearn Research and AnalyticsLearn Business CommunicationLearn Business AnalyticsLearn Statistics for Data ScienceLearn Deep LearningLearn TableauLearn SAS ProgrammingLearn SQL for Data AnalyticsLearn Clinical Trial Analysis &amp; ReportingLearn Natural Language ProcessingLearn Data ScienceWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 17th Jul'25 and 21st Aug'25                                    3. are available for duration of 2 months                                    4. are from Jaipur only                                    5. have relevant skills and interests                    * Women wanting to start/restart their career can also apply.Other requirements                    1. Have completed BBA or MBA                                    2. Prior experience in terms of projects/internships in Market research are PREFERRED.                PerksCertificate Letter of recommendation Informal dress codeNumber of openings        2                        About Lohagarh Software Solutions Pvt Ltd                        Lohagarh Software Solutions is a start-up with a mission to empower students with informed education and career decisions, aligning their choices with their inherent strengths, and offering continuous mental well-being support to students and their parents.Every year, around 200,000 students enrol in coaching hubs like Kota, Jaipur, and Sikar to prepare for competitive exams such as IIT-JEE and NEET. Students endure immense academic pressure that often leads to stress, mental health challenges, and the loss of formative years. Many students enrol in coaching programs without a clear understanding of their aptitudes, strengths, or long-term career goals, resulting in disengagement, frustration, bad health, and loss of time.We aim to help Students in these areas.Activity on InternshalaHiring since May 20252 opportunities posted2 candidates hired                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -716,24 +716,24 @@
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:15</t>
+          <t>2025-07-20 10:40:57</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/design-communication-internship-in-mumbai-at-movi-ecoserve-private-limited1751519202</t>
+          <t>https://internshala.com/internship/detail/market-research-internship-in-jaipur-at-lohagarh-software-solutions-pvt-ltd1752812739</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>HR Generalist</t>
+          <t>Field Sales</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>About the work from home job/internship    Selected intern's day-to-day responsibilities include: 1. Provide tailored guidance to professionals in managing their job applications, enhancing LinkedIn profiles, and improving interview readiness to ensure a smooth and engaging candidate experience.2. Analyze labor market trends, industry shifts, and employer requirements to provide strategic input that supports both talent development and internal HR planning.3. Monitor employee and candidate engagement throughout the hiring process, evaluate outcomes, and use feedback to fine-tune HR strategies and enhance overall service quality.4. Work closely with employees, candidates, and cross-functional teams to implement initiatives that improve HR services, boost operational efficiency, and foster a positive experience across all touchpoints.Skill(s) requiredEffective CommunicationEnglish Proficiency (Written)LinkedIn MarketingTime ManagementEarn certifications in these skillsLearn Business CommunicationLearn Human Resource ManagementWho can applyOnly those candidates can apply who:                1. are available for the work from home job/internship                                    2. can start the work from home job/internship between 15th Jul'25 and 19th Aug'25                                    3. are available for duration of 2 months                                    4. have relevant skills and interests                    * Women wanting to start/restart their career can also apply.PerksCertificate Letter of recommendation Flexible work hoursNumber of openings        20                        About NxtJob                Website         At NxtJob, we are at the intersection of two rapidly growing industries - AI and online consulting/coaching. We've built an AI-powered web app and consulting program tailored to help job seekers land their ideal roles. Our mission is straightforward yet impactful: to empower professionals to showcase their skills and secure the salaries they deserve. It's why we're called NxtJob. Over 1,400 professionals have already used our services to land high-paying job offers around the world. In just 18 months of operations, we've achieved exceptional growth, consistently delivering outstanding results for our clients. As we continue to expand, we're looking for passionate team members to join us on this journey of transformation and empowerment.    Activity on InternshalaHiring since December 202373 opportunities posted181 candidates hired                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
+          <t>About the internship    Key Responsibilities:1. Understand and explain the key features and benefits of our IT product.2. Conduct on-field visits to potential clients across Pithampur, Dewas Naka, and Indore.3. Assist in generating leads and identifying new business opportunities.Participate in client meetings, demos, and follow-ups.4. Collect insights from field visits and share feedback with the internal team.5. Maintain proper records of leads, interactions, and daily activities.Skill(s) requiredBusiness DevelopmentClient InteractionEnglish Proficiency (Spoken)Field SalesField WorkHindi Proficiency (Spoken)Lead GenerationNegotiationSalesEarn certifications in these skillsLearn Business CommunicationLearn Digital MarketingLearn Business AnalyticsWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 11th Jul'25 and 15th Aug'25                                    3. are available for duration of 3 months                                    4. are from Indore only                                    5. have relevant skills and interests                    Other requirements                    1. Good communication and interpersonal skills                                    2. Interest in technology and willingness to learn about IT products                                    3. Self-motivated, proactive, and comfortable with field work                                    4. Basic knowledge of sales or marketing is a plus                                    5. Ability to travel locally for field visits                PerksCertificateAdditional informationStipend Structure:Fixed pay: ₹ 8,000 - 10,000 /month                    Incentive pay: ₹ 2,000 - 20,000 /month                     Number of openings        4                        About BluCursor Infotech Private Limited                Website         bluCursor Infotech Private Limited is a government-certified and acclaimed IT company. Established in 2013, we have fulfilled the needs of a diverse range of clients belonging to various countries and have been flourishing since. bluCursor Infotech Private Limited consists of technology evangelists, full-stack consumers, and web solution experts. Our offerings include SOA-based applications, big data solutions, and mobile applications. We have a well-established track record and our services have always ensured great customer satisfaction.     Activity on InternshalaHiring since April 20234 opportunities posted                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -751,24 +751,24 @@
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:16</t>
+          <t>2025-07-20 10:40:57</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/work-from-home-hr-generalist-internship-at-nxtjob1752565321</t>
+          <t>https://internshala.com/internship/detail/field-sales-internship-in-indore-at-blucursor-infotech-private-limited1752237511</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Web3- Social Media Marketing</t>
+          <t>Sales and Marketing</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>About the work from home job/internship    Selected intern's day-to-day responsibilities include:1. Content creation: Write, schedule, and publish daily tweets, threads, memes, and replies that match the brand's tone and resonate with our audience.2. Brand voice: Develop and maintain a distinct, authentic, and engaging voice for the brand on Twitter.3. Community engagement: Reply to mentions, join conversations, participate in trending hashtags, and build relationships with key community members and influencers.4. Trendspotting: Monitor Web3, crypto, and Twitter trends to create relevant, timely, and viral content.5. Performance tracking: Monitor analytics (engagement, reach, followers), report on campaign results, and optimize strategy based on data.6. Collaboration: Coordinate with content, design, and marketing teams to ensure posts align with wider campaigns and brand initiatives.7. Creative campaigns: Propose and execute campaigns like giveaways, AMAs, polls, and collaborations with other Twitter accounts.Skill(s) requiredCreative WritingEnglish Proficiency (Spoken)English Proficiency (Written)Earn certifications in these skillsLearn Creative WritingLearn Business CommunicationLearn Digital MarketingLearn Business AnalyticsWho can applyOnly those candidates can apply who:                1. are available for the work from home job/internship                                    2. can start the work from home job/internship between 12th Jul'25 and 16th Aug'25                                    3. are available for duration of 3 months                                    4. have relevant skills and interests                    * Women wanting to start/restart their career can also apply.PerksCertificate Letter of recommendation Flexible work hoursNumber of openings        2                        About Podha Protocol                        Podha Protocol is a web3 yield generation platform via real real-world digital asset management company. Recognized as a top-tier digital asset yield platform, Podha delivers reliable and forward-thinking yield solutions that bolster the digital asset economy.    Activity on InternshalaHiring since May 202515 opportunities posted                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
+          <t>About the internship    Selected intern's day-to-day responsibilities include: 1. Assist in identifying and onboarding new restaurants, cloud kitchens, and cafes to the Restomart platform2. Conduct field visits across Chennai to understand customer pain points and recommend relevant product bundles3. Support order placement and fulfillment coordination via WhatsApp and internal systems. Prepare performance reports, track leads, and maintain CRM disciplineSkill(s) requiredBusiness DevelopmentCanvaDigital MarketingTamil Proficiency (Spoken)Earn certifications in these skillsLearn Email MarketingLearn Facebook MarketingLearn Google AdWordsLearn Search Engine MarketingLearn SEOLearn Social Media MarketingWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 17th Jul'25 and 21st Aug'25                                    3. are available for duration of 3 months                                    4. are from Chennai only                                    5. have relevant skills and interests                    PerksCertificate Letter of recommendation Informal dress codeAdditional informationStipend Structure:Fixed pay: ₹ 6,000 - 8,000 /month                    Incentive pay: ₹ 4,000 - 6,000 /month                     Number of openings        2                        About Restomart                Website         We're a one-stop B2B platform powering restaurants and cafes with quality food supplies and next-day delivery. Bootstrapped and profitable, we're now scaling our platform, category offerings, and operations to build the "OS for restaurants" solving for procurement, inventory, recipe costing, and beyond.    Activity on InternshalaHiring since June 20252 opportunities posted                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -778,7 +778,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Web Development Internship</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
@@ -786,24 +786,24 @@
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:16</t>
+          <t>2025-07-20 10:40:58</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/work-from-home-web3-social-media-marketing-internship-at-podha-protocol1752338082</t>
+          <t>https://internshala.com/internship/detail/sales-and-marketing-internship-in-chennai-at-restomart1752752843</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Management Trainee</t>
+          <t>Video Editing/Making</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>About the work from home job/internship    Selected intern's day-to-day responsibilities include: 1. Support professionals in enhancing their job search approach by improving personal branding strategies, such as optimizing LinkedIn profiles and aligning career goals with current hiring trends.2. Conduct detailed research on evolving job market patterns, industry shifts, and employer recruitment behaviors to inform internal strategies and client advisory.3. Monitor and analyze job application metrics, track client journey progress, and generate insights to boost placement and conversion rates.4. Assist in improving internal operations by identifying inefficiencies, recommending workflow enhancements, and supporting implementation of process improvements.5. Collaborate with cross-functional teams to co-create and implement innovative operational solutions aimed at elevating the overall client and stakeholder experience.Skill(s) requiredEffective CommunicationEnglish Proficiency (Written)LinkedIn MarketingTime ManagementEarn certifications in these skillsLearn Business CommunicationLearn Business AnalyticsLearn Digital MarketingLearn Human Resource ManagementWho can applyOnly those candidates can apply who:                1. are available for the work from home job/internship                                    2. can start the work from home job/internship between 15th Jul'25 and 19th Aug'25                                    3. are available for duration of 2 months                                    4. have relevant skills and interests                    * Women wanting to start/restart their career can also apply.PerksCertificate Letter of recommendation Flexible work hoursNumber of openings        20                        About NxtJob                Website         At NxtJob, we are at the intersection of two rapidly growing industries - AI and online consulting/coaching. We've built an AI-powered web app and consulting program tailored to help job seekers land their ideal roles. Our mission is straightforward yet impactful: to empower professionals to showcase their skills and secure the salaries they deserve. It's why we're called NxtJob. Over 1,400 professionals have already used our services to land high-paying job offers around the world. In just 18 months of operations, we've achieved exceptional growth, consistently delivering outstanding results for our clients. As we continue to expand, we're looking for passionate team members to join us on this journey of transformation and empowerment.    Activity on InternshalaHiring since December 202373 opportunities posted181 candidates hired                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
+          <t>About the internship    We are seeking a talented video editing expert who possesses advanced skills in utilizing the latest AI tools to create engaging short marketing videos. The ideal candidate should have a keen eye for detail, creativity, and proficiency in editing software.Selected intern's day-to-day responsibilities include: 1. Collaborate with the marketing team to understand project requirements and objectives.2. Utilize cutting-edge AI tools to enhance video content and create captivating marketing videos.3. Edit raw footage, adding effects, transitions, graphics, and sound to produce high-quality videos.4. Ensure videos align with brand guidelines and maintain consistency in style and tone.5. Optimize videos for various platforms, including social media channels, websites, and presentations.6. Stay updated on industry trends and emerging technologies to incorporate innovative techniques into video editing processes.7. Manage multiple projects simultaneously and adhere to deadlines.8. Provide constructive feedback and contribute to brainstorming sessions for creative ideas.Skill(s) requiredAdobe IllustratorAdobe PhotoshopVideo EditingVideo MakingEarn certifications in these skillsLearn Adobe PhotoshopLearn Adobe Premiere ProLearn Video EditingWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 3rd Jul'25 and 7th Aug'25                                    3. are available for duration of 3 months                                    4. are from Chennai only                                    5. have relevant skills and interests                    Other requirements                    1. Proficiency in video editing software such as Adobe Premiere Pro, Final Cut Pro, or similar tools.                                    2. Demonstrated expertise in using AI tools for video editing and enhancement.                                    3. Strong understanding of storytelling techniques and visual aesthetics..                                    4. Demonstrated expertise in using AI tools for video editing and enhancement.                                    5. Strong understanding of storytelling techniques and visual aesthetics.                                    6. A freelancer can also apply for the internship.                PerksCertificate Letter of recommendationAdditional information                1. Candidates may be required to provide a portfolio showcasing their previous work.2. The position offers opportunities for professional growth and development within the company.                Number of openings        1                        About MiTran Global                Website         We are a global organization focusing on delivering world-class tools to understand the mindset of students and provide them with appropriate training courses.    Activity on InternshalaHiring since October 202229 opportunities posted                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -821,24 +821,24 @@
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:17</t>
+          <t>2025-07-20 10:40:59</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/work-from-home-management-trainee-internship-at-nxtjob1752565361</t>
+          <t>https://internshala.com/internship/detail/video-editing-making-internship-in-chennai-at-mitran-global1751542350</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>UI/UX Design</t>
+          <t>Kannada Audio Recording Expert (Native Speakers)</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>About the internship    As a UI/UX Design intern, you will have the opportunity to work on cutting-edge projects and gain hands-on experience in the field. Your creativity and skills in Wireframing, UI and UX Design, Figma, Sketch, and Adobe Illustrator will be put to the test as you collaborate with our team to create user-friendly interfaces for our digital platforms.Key Responsibilities:1. Collaborate with the product officer to create wireframes and prototypes for new features and enhancements.2. Conduct user research and testing to gather insights and feedback for design improvements.3. Work closely with developers to ensure designs are implemented accurately and efficiently.4. Create visually appealing and intuitive designs that enhance the overall user experience.5. Stay up-to-date with the latest design trends and technologies to continually improve our products.6. Assist in the creation of design assets and style guides to maintain brand consistency.7. Participate in design reviews and provide constructive feedback to help refine design concepts. If you are a motivated and creative individual looking to jumpstart your career in UI/UX design, we want to hear from you! Join us and be part of a dynamic team that is shaping the future.Skill(s) requiredAdobe IllustratorFigmaSketchUI &amp; UX DesignWireframingEarn certifications in these skillsLearn FigmaLearn Rapid PrototypingLearn UI &amp; UX DesignLearn WireframingWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 18th Jul'25 and 22nd Aug'25                                    3. are available for duration of 2 months                                    4. are from Coimbatore only                                    5. have relevant skills and interests                    PerksCertificate Letter of recommendation Flexible work hours Informal dress codeNumber of openings        1                        About HiFresh Agro Private Limited                        HiFresh Agro Private Limited is a startup focused on producing protein-rich food such as mushrooms and Spirulina, with strategic plans to expand into the export business of agricultural products such as millets, coir, and other agricultural produce where there is a demand.    Activity on InternshalaHiring since June 202415 opportunities posted8 candidates hired                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
+          <t>About the work from home job/internship    We are currently looking for fluent Kannada speakers to participate in an ongoing audio recording project. If you have strong verbal communication skills, a keen eye for detail, and are proficient in Kannada, this is a great opportunity for you.Selected intern's day-to-day responsibilities include:1. Recording audio on assigned topics with clear and fluent Kannada pronunciation.2. Speaking exclusively in Kannada throughout all recordings.3. Staying on topic and following the given subpoints without deviating from the script.4. Using the specified mobile application to complete recordings.5. Ensuring recordings are done in a quiet, noise-free environment for optimal audio quality.6. Maintaining a stable internet connection and staying fully focused   no multitasking during sessions.7. Adhering to professional standards: avoiding offensive, abusive, or discriminatory language, and refraining from sharing any personal information.Note: 1.  Each participant will record 220 short phrases provided on the platform.2. This is a one-time task, and all recordings will be completed through a mobile. Application.Skill(s) requiredCreative WritingEnglish Proficiency (Spoken)English Proficiency (Written)Kannada Proficiency (Spoken)Kannada Proficiency (Written)ProofreadingVoice-over artistEarn certifications in these skillsLearn Creative WritingLearn Business CommunicationLearn FrenchWho can applyOnly those candidates can apply who:                1. are available for the work from home job/internship                                    2. can start the work from home job/internship between 20th Jul'25 and 24th Aug'25                                    3. are available for duration of 1 week                                    4. have relevant skills and interests                    * Women wanting to start/restart their career can also apply.Other requirements                    1. Fluency in Kannada.                                    2. Excellent reading and speaking skills in the Kannada Language.                                    3. Ability to commit to a minimum of 3-4 hours per day.                                    4. Strong attention to detail and ability to meet project specifications.                PerksCertificate Flexible work hoursNumber of openings        20                        About Solvitude                LinkedIn page         Solvitude is a rapidly growing content service platform where users get various academic and content writing services like article writing, textbook solutions, essay writing, translations, and many more. Solvitude has the perfect team of experts for such work. The team adheres to and fulfills the needs of the clients. Various leading companies in the ed-tech industry outsource their writing requirements to us. By doing so, they get the benefits of one of the most capable content writing services online. Join our yoga centre team at Solvitude.    Activity on InternshalaHiring since April 2023370 opportunities posted84 candidates hired                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -856,24 +856,24 @@
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:18</t>
+          <t>2025-07-20 10:40:59</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/ui-ux-design-internship-in-coimbatore-at-hifresh-agro-private-limited1752838475</t>
+          <t>https://internshala.com/internship/detail/work-from-home-part-time-kannada-audio-recording-expert-native-speakers-internship-at-solvitude1752995847</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Digital Marketing</t>
+          <t>UI/UX Design</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>About part time job/internship    Selected intern's day-to-day responsibilities include: 1. Assisting in digital marketing activities and campaign execution2. Managing and growing social media platforms through engaging content3. Supporting branding and advertising initiatives for better visibility4. Performing basic search engine optimization (SEO) tasks to improve rankings5. Creating graphics and visual content for marketing purposes6. Helping run and monitor search engine marketing (SEM) campaigns7. Managing Digital Channels8. Content Creation and Management9. Website Optimization:10. Improving website visibility through SEO (Search Engine Optimization) and content marketing strategies.  11. Campaign Management: Managing and optimizing digital advertising campaigns across various platforms like Google Ads, social media, and email marketing.  12. Technical Proficiency: Familiarity with web analytics tools (e.g., Google Analytics), content management systems (CMS), and other digital marketing tools.  Skill(s) requiredDigital MarketingEmail MarketingFacebook MarketingInstagram MarketingSearch Engine Marketing (SEM)Search Engine Optimization (SEO)Social Media MarketingEarn certifications in these skillsLearn Email MarketingLearn Facebook MarketingLearn Google AdWordsLearn Search Engine MarketingLearn SEOLearn Social Media MarketingWho can applyOnly those candidates can apply who:                1. are available for the part time job/internship                                    2. can start the part time job/internship between 18th Jul'25 and 22nd Aug'25                                    3. are available for duration of 4 months                                    4. are from Bangalore only                                    5. have relevant skills and interests                    * Women wanting to start/restart their career can also apply.Other requirements                    1. Assisting in digital marketing activities and campaign execution                                    2. Managing and growing social media platforms through engaging content                                    3. Supporting branding and advertising initiatives for better visibility                                    4. Performing basic search engine optimization (SEO) tasks to improve rankings                                    5. Creating graphics and visual content for marketing purposes                                    6. Helping run and monitor search engine marketing (SEM) campaigns                PerksCertificate Letter of recommendation Flexible work hoursNumber of openings        5                        About Varuna                        Varuna is a trusted name in the field of water and wastewater management, offering innovative, sustainable, and cost-effective solutions across India. Headquartered in Bangalore, we specialize in the design, manufacturing, installation, and maintenance of high-quality Sewage Treatment Plants (STP), Effluent Treatment Plants (ETP), Water Treatment Plants (WTP), Modular Precast RCC Tanks, Water Softeners, and Rainwater Harvesting Systems.                            Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
+          <t>About the internship    Selected intern's day-to-day responsibilities include:1. Create low and high-fidelity wireframes and prototypes.2. Develop user flows and information architecture to enhance usability.3. Design responsive and adaptive UI for mobile and web applications.4. Work with typography, color theory, and visual hierarchy to create aesthetically pleasing designs.5. Utilize Figma for design systems, auto-layout, variants, and prototyping.6. Collaborate with developers and stakeholders to refine design solutionsSkill(s) requiredFigmaEarn certifications in these skillsLearn FigmaLearn UI &amp; UX DesignWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 20th Jul'25 and 24th Aug'25                                    3. are available for duration of 6 months                                    4. are from Jaipur only                                    5. have relevant skills and interests                    Number of openings        10                        About EG Allied Private Limited                        Entire Globe Allied is in the IT services &amp; BPO industry. We offer our services globally and connect you to the world of innovation. We believe in providing the best solution to our clients by keeping the customer's satisfaction and the brand's reputation in mind. We frame our work with innovative ideas to get ahead of the global competition, which also helps us to provide our clients with high-quality services. We provide services in IT, customer engagement, accounting, and digital marketing.    Activity on InternshalaHiring since June 2021222 opportunities posted4 candidates hired                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -891,24 +891,24 @@
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:18</t>
+          <t>2025-07-20 10:41:00</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/part-time-digital-marketing-internship-in-bangalore-at-varuna1752840350</t>
+          <t>https://internshala.com/internship/detail/ui-ux-design-internship-in-jaipur-at-eg-allied-private-limited1752984633</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Finance Research Analyst</t>
+          <t>Content and Social Media Marketing</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>About the work from home job/internship    Selected intern's day-to-day responsibilities include:1. Participate in internal training sessions or knowledge-sharing activities2. Track stock market trends, economic indicators, and global financial news3. Conduct research on listed companies, market sectors, and industriesSkill(s) requiredFinancial literacyEarn certifications in these skillsLearn Stocks and TradingLearn Business CommunicationLearn Business AnalyticsLearn Financial modeling valuationLearn Personal FinanceWho can applyOnly those candidates can apply who:                1. are available for the work from home job/internship                                    2. can start the work from home job/internship between 18th Jul'25 and 22nd Aug'25                                    3. are available for duration of 1 month                                    4. have relevant skills and interests                    * Women wanting to start/restart their career can also apply.PerksCertificate Letter of recommendation Flexible work hoursNumber of openings        20                        About Savvy Merit                Website         Savvy Merit is a forward-thinking educational company committed to empowering individuals with the knowledge, tools, and strategies needed to thrive in the world of finance and the stock market. Our mission is to simplify complex financial concepts and make investing accessible to everyone, from curious beginners to aspiring market professionals. We offer high-quality education through structured courses, live mentorship, interactive workshops, and market insights. Our expert-led curriculum covers a wide range of topics, including stock market fundamentals, technical and fundamental analysis, portfolio management, and financial planning, all with a focus on real-world applications. What sets us apart is our team of experienced mentors, beginner-to-advanced learning tracks, live market training and simulations, strong community support, engaging webinars, and access to up-to-date tools and resources.    Activity on InternshalaHiring since June 202559 opportunities posted                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
+          <t>About the internship    Are you a creative individual with a passion for content creation and social media marketing? Homemade Love is seeking a talented Content and Social Media Marketing intern to join our team! As a key member of our marketing team, you will have the opportunity to showcase your skills in video editing, social media marketing, Instagram marketing, and videography. Key Responsibilities:1. Create engaging and visually appealing video content for our social media channels2. Develop and implement social media marketing strategies to increase brand awareness3. Manage and grow our Instagram presence through creative and innovative content4. Collaborate with the marketing team to brainstorm and execute new ideas for content5. Assist in capturing high-quality video footage for promotional purposes6. Analyze and report on social media performance metrics to optimize marketing efforts7. Stay up-to-date on industry trends and best practices to continuously improve our marketing strategies If you are a self-motivated individual with a strong eye for detail and a love for all things creative, we want to hear from you! Join us at Homemade Love and make a real impact on our brand's digital presence. Apply now and show us what you've got!Skill(s) requiredInstagram MarketingSocial Media MarketingVideo EditingVideographyEarn certifications in these skillsLearn Adobe Premiere ProLearn Facebook MarketingLearn Social Media MarketingLearn Video EditingWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 20th Jul'25 and 24th Aug'25                                    3. are available for duration of 3 months                                    4. are from Delhi only                                    5. have relevant skills and interests                    * Women wanting to start/restart their career can also apply.PerksInformal dress codeNumber of openings        2                        About Homemade Love LLP                        We're a homegrown pickle, chutney, and traditional recipe brand. We are very particular about delivering quality products like a true Punjabi mom, and careful to make only small quantities of Jams and pickles, slow-cooked with love and perfectly simmered. Wanting to cater to all kinds of preferences, we laid a strong emphasis on producing only unadulterated all-natural pickles and jams, made from locally sourced vegetables, simmered in pure oils and vinegar. Only natural preservatives like lemon, mustard oil, vinegar, and sugar are used to create products that are made to last for 8-12 months with refrigeration and 6 months - without. Willing to ship fresh batches of pickles and jams to just about anywhere, we make sure that each bottle packed is filled to the brim with the product and the love.    Activity on InternshalaHiring since August 202210 opportunities posted                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -926,24 +926,24 @@
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:19</t>
+          <t>2025-07-20 10:41:00</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/work-from-home-part-time-finance-research-analyst-internship-at-savvy-merit1752841432</t>
+          <t>https://internshala.com/internship/detail/content-and-social-media-marketing-internship-in-delhi-at-homemade-love-llp1752989543</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Project Management</t>
+          <t>Graphic Design</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>About the internship    As a Project Management intern at VerboLabs, you will have the opportunity to work in a dynamic and fast-paced environment where your skills in Interpersonal communication, Effective Communication, and Time Management will be put to the test. Your role will involve collaborating with team members, clients, and vendors to ensure projects are completed successfully and on time. Key responsibilities:1. Assist in creating project plans and timelines2. Communicate project updates and progress to all stakeholders3. Coordinate with team members to delegate tasks and ensure deadlines are met4. Conduct research and analysis to support project objectives5. Assist in identifying potential risks and developing mitigation strategies6. Participate in meetings and provide input on project strategy and direction7. Maintain project documentation and ensure accuracy and completeness of recordsIf you are a proactive and driven individual looking to gain hands-on experience in project management, this internship is the perfect opportunity to expand your skills and make a real impact. Apply now and take the first step towards a rewarding career in project management at VerboLabs.Skill(s) requiredEffective CommunicationInterpersonal skillsTime ManagementEarn certifications in these skillsLearn Business CommunicationWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 18th Jul'25 and 22nd Aug'25                                    3. are available for duration of 3 months                                    4. are from Udaipur only                                    5. have relevant skills and interests                    * Women wanting to start/restart their career can also apply.PerksCertificate Letter of recommendation Job offerAdditional informationJob offer: On successful conversion to a permanent employee, the candidate can expect a salary of ₹ 240000 to 300000/year Number of openings        4                        About VerboLabs                LinkedIn page         VerboLabs is a leading language services company based in Bangalore, India. We are one of the top website &amp; human translation service providing agencies. Our great base of experienced native translators makes sure that every project is taken up sincerely and that the best efforts are put in to make it stand out in terms of quality.    Activity on InternshalaHiring since November 20226 opportunities posted                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
+          <t>About part time job/internship    Selected intern's day-to-day responsibilities include:1. Design the layout of essential business materials (e.g. business cards, presentations)2. Create infographics and presentation materials to simplify the communication of complex concepts and data3. Work on editing video clips for use on social media platformsNotes: 1. Windows is not accepted due to the nature of the work, you have to work on a MacBook.2. If you perform well, you might be working very closely with our marketing and founding teams to showcase your creativity at its best.Skill(s) requiredAdobe IllustratorAdobe PhotoshopCorelDRAWSketchEarn certifications in these skillsLearn Adobe PhotoshopLearn Graphic DesignLearn AnimationLearn Video EditingWho can applyOnly those candidates can apply who:                1. are available for the part time job/internship                                    2. can start the part time job/internship between 19th Jul'25 and 23rd Aug'25                                    3. are available for duration of 3 months                                    4. are from Mohali only                                    5. have relevant skills and interests                    Other requirements                    1. The candidate should have a MacBook/Mac Mini (only Macintosh OS), which is required for internal processes.                                    2. The candidate should be eager to learn about creativity and test it within brand guidelines.                PerksCertificate Letter of recommendation Informal dress code 5 days a week Free snacks &amp; beverages Job offerAdditional informationJob offer: On successful conversion to a permanent employee, the candidate can expect a salary of ₹ 200000 to 240000/year Number of openings        5                        About Alphanumeric Ideas Private Limited                        We deal in digital empowerment and promotion solutions and have been accredited as one of APAC's top digital marketing agencies. We are a Google premier partner agency listed among the top 3% of companies in the APAC region. We have been working with leading brands like The Whole Truth Foods, and Agarwal Packers &amp; Movers, to name a few.    Activity on InternshalaHiring since January 2020946 opportunities posted45 candidates hired                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -961,24 +961,24 @@
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:20</t>
+          <t>2025-07-20 10:41:01</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/project-management-internship-in-udaipur-at-verbolabs1752837603</t>
+          <t>https://internshala.com/internship/detail/part-time-graphic-design-internship-in-mohali-at-alphanumeric-ideas-private-limited1752900107</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Telecalling / Customer Service</t>
+          <t>Marketing</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>About the internship    Selected intern's day-to-day responsibilities include: 1. Make cold calls and follow-ups with customers and prospects2. Handle product, order, and service-related queries via phone, email, and WhatsApp3. Maintain accurate call logs and feedback records4. Coordinate with internal teams to ensure smooth customer service5. Assist with customer complaints, returns, and status updates6. Create and manage basic reports in ExcelSkill(s) requiredAdaptabilityAttention to DetailCollaborationComputer skillsCoordinationDocument ManagementEffective CommunicationReport WritingEarn certifications in these skillsLearn MS-ExcelLearn Business CommunicationLearn Digital MarketingLearn Business AnalyticsWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 18th Jul'25 and 22nd Aug'25                                    3. are available for duration of 3 months                                    4. are from Kolkata only                                    5. have relevant skills and interests                    Other requirements                    1. Students or freshers based in Kolkata                                    2. Strong verbal communication in English, Hindi, and Bengali                                    3. Confident in handling phone calls and cold outreach                                    4. Well-versed in MS Excel, email, and WhatsApp tools                                    5. Friendly, composed, and detail-oriented                PerksCertificateNumber of openings        4                        About Anuschka Leather-India Private Limited                Website         Anuschka is a premium fashion brand renowned for having the world's largest collection of hand-painted bags. Headquartered in the USA, it sells across North America, Europe, Australia, and the UK, with its Sales and Marketing unit in India. The brand name means "like no other", and for over 36 years, Anuschka has empowered artisans to create wearable art that tells stories and supports their families. As part of the Anuschka family, you contribute to a global circle of empowerment, connecting art lovers and artisans through storytelling, creativity, and community. For more details-  www.anuschkaleather.com    Activity on InternshalaHiring since May 202525 opportunities posted                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
+          <t>About the internship    Selected intern's day-to-day responsibilities:1. Assist in integrating ERP platforms and professional service ecosystems to enhance compliance, tax intelligence, and reconciliation workflows2. Support the team in showcasing SaaS solutions for accounting, finance, tax compliance, and risk management3. Create engaging content for social media platforms (LinkedIn, Facebook, YouTube)4. Help with client connect initiatives (email campaigns, webinars, events)5. Assist in implementing SaaS tools to streamline client processes6. Collaborate with teams to support platform sales and handle routine platform-related queries7. Collect and share client feedback with product development teamsSkill(s) requiredDigital MarketingEmail MarketingEnglish Proficiency (Spoken)English Proficiency (Written)FinanceSales StrategySocial Media MarketingEarn certifications in these skillsLearn Business CommunicationLearn Email MarketingLearn Facebook MarketingLearn Google AdWordsLearn Search Engine MarketingLearn SEOLearn Social Media MarketingLearn Financial ModelingLearn TallyLearn Stocks and TradingWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 19th Jul'25 and 23rd Aug'25                                    3. are available for duration of 4 months                                    4. are from Chennai only                                    5. have relevant skills and interests                    Other requirements                    1. Bachelor's degree in accounting, finance, law, business administration, or related fields                                    2. Strong interest in SaaS solutions, accounting, and finance                                    3. Good knowledge of social media platforms and content creation                PerksCertificate Letter of recommendationNumber of openings        1                        About Gigart Solutions Private Limited                        We are a freelancing marketplace focused on providing technology-enabled platform services that ensure the availability of professionals on a short-term basis. The service is expected to be offered to the right person at the right time and at the right cost. This service saves on employing such resources on a full-time basis.    Activity on InternshalaHiring since January 202143 opportunities posted8 candidates hired                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -996,24 +996,24 @@
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:20</t>
+          <t>2025-07-20 10:41:02</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/telecalling-customer-service-internship-in-kolkata-at-anuschka-leather-india-private-limited1752838563</t>
+          <t>https://internshala.com/internship/detail/marketing-internship-in-chennai-at-gigart-solutions-private-limited1752911509</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Law/Legal</t>
+          <t>Business Development (Sales)</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>About the internship    Selected intern's day-to-day responsibilities include:1. Conduct legal research and analysis on various matters2. Draft legal documents, contracts, and agreements3. Assist in preparing for court hearings and trials4. Review and analyze legal documents and correspondence5. Communicate with clients, attorneys, and other legal professionals6. Maintain and organize legal files and documentation7. Provide support to the legal team as neededAny other cross-functional team support if requiredSkill(s) requiredEnglish Proficiency (Spoken)English Proficiency (Written)MS-OfficeMS-WordEarn certifications in these skillsLearn Business CommunicationLearn MS-ExcelWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 18th Jul'25 and 22nd Aug'25                                    3. are available for duration of 6 months                                    4. have relevant skills and interests                    Other requirements                    This role is not open to freshers; we require candidates with relevant experience.                                    The stipend will be based on the candidate’s skills and prior experience.                Number of openings        2                        About Movi Ecoserve Private Limited                        Movi Ecoserve works in sustainable technologies. We work majorly with the government and municipalities in pan India.     Activity on InternshalaHiring since February 202261 opportunities posted3 candidates hired                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
+          <t>About the internship    Key responsibilities:1. Contact potential students and organizations via calls, emails, and social media to describe GradX programs and career opportunities2. Schedule and conduct counseling sessions or product demos with interested candidates online or in person as needed3. Track and manage a pipeline of leads using CRM tools or spreadsheets, ensuring regular follow-up and engagement4. Monitor progress towards weekly and monthly sales targets and adjust strategies to improve conversion rates5. Work consistently to achieve and exceed assigned weekly and monthly sales targets for enrollments and partnerships6. Collect insights and feedback from prospects and enrolled clients regarding course offerings and service quality to inform improvements7. Provide prompt support and ongoing communication to address queries and maintain strong follow-up throughout the enrollment cycle8. Collaborate with marketing, academic, and placement teams to ensure a seamless onboarding experience and alignment of objectives9. Maintain clear records of activity, customer interactions, and sales outcomes, and submit reports to team leaders10. Participate in team meetings, strategy sessions, and training programs to improve performance and enhance product knowledgeSkill(s) requiredClient Relationship Management (CRM)Effective CommunicationEnglish Proficiency (Spoken)English Proficiency (Written)Interpersonal skillsSalesSales StrategyEarn certifications in these skillsLearn Business CommunicationLearn Digital MarketingLearn Business AnalyticsWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 19th Jul'25 and 23rd Aug'25                                    3. are available for duration of 5 months                                    4. are from Pune only                                    5. have relevant skills and interests                    * Women wanting to start/restart their career can also apply.Other requirements                    1. Bachelor’s degree (business, marketing, or related field preferred)                                    2. Sales or business development experience (preferably EdTech)                                    3. Excellent communication and interpersonal skills                                    4. Experience with CRM tools and digital outreach                                    5. Strong organizational and multitasking abilities                                    6. Target-driven and self-motivated                                    7. Quick learner, adaptable to change                                    8. Customer-focused attitude                                    9. Team player                PerksCertificate Letter of recommendation Informal dress code Job offerAdditional informationStipend Structure:Fixed pay: ₹ 5,000 - 10,000 /month                    Incentive pay: ₹ 8,000 - 30,000 /month                     Job offer: On successful conversion to a permanent employee, the candidate can expect a salary of ₹ 300000 to 600000/year Number of openings        6                        About GradX Academy                Website         GradX Academy is a next-generation EdTech platform on a mission to bridge the skill gap between traditional education and the real-world tech industry. We specialize in delivering high-impact training programs in salesforce, data cloud, marketing cloud, business development, and other in-demand technologies. Our courses are designed and delivered by industry experts with a focus on practical learning, real-time projects, and career transition support. We've helped hundreds of professionals and students land high-paying jobs and accelerate their careers in IT, even without prior tech backgrounds. At GradX Academy, we believe in "Learning by Doing." Join us to be part of a fast-growing team that's shaping the future of tech education and empowering the next generation of IT leaders.Activity on InternshalaHiring since July 20252 opportunities posted                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1031,24 +1031,24 @@
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:21</t>
+          <t>2025-07-20 10:41:02</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/law-legal-internship-in-mumbai-at-movi-ecoserve-private-limited1752834353</t>
+          <t>https://internshala.com/internship/detail/business-development-sales-internship-in-pune-at-gradx-academy1752919512</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Human Resources (HR)</t>
+          <t>Law/Legal</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>About the internship    Position: HR InternLocation: Jaipur (Onsite)Shift Timing: Day Shift (10:00 AM to 7:00 PM)Stipend:    15,000 per monthAbout the Role:We are looking for a motivated and enthusiastic HR Intern to join our team at our Jaipur office. This is a great opportunity for individuals who are passionate about building a career in human resources and wish to gain hands-on experience in a professional setting.Key Responsibilities:Assist in recruitment processes, including sourcing, screening, and scheduling interviews.Maintain and update employee records and HR databases.Support onboarding and orientation processes for new hires.Help in organizing employee engagement activities and events.Provide support for daily HR operations and administrative tasks.Handle documentation and assist in policy compliance.Requirements:Pursuing or recently completed a degree in Human Resources, Business Administration, or a related field.Strong communication and interpersonal skills.Proficiency in MS Office (Word, Excel, PowerPoint).Ability to multitask and prioritize tasks efficiently.Positive attitude and eagerness to learn.Skill(s) requiredEnglish Proficiency (Spoken)English Proficiency (Written)MS-ExcelMS-WordRecruitmentEarn certifications in these skillsLearn Business CommunicationLearn MS-ExcelLearn about RecruitmentWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 18th Jul'25 and 22nd Aug'25                                    3. are available for duration of 4 months                                    4. are from Jaipur only                                    5. have relevant skills and interests                    PerksCertificate Letter of recommendation Flexible work hours 5 days a weekNumber of openings        1                        About Softsensor.ai                Website         Softsensor.ai is a USA and India-based corporation focused on delivering outcomes to clients using data. Our expertise lies in a collection of people, methods, and accelerators to rapidly deploy solutions for our clients. Our principals have significant experience with leading global consulting firms &amp; corporations and delivering large-scale solutions. We are focused on data science and analytics for improving the process and organizational performance. We are working on cutting-edge data science technologies like NLP, CNN, and RNN and applying them in the business context.    Activity on InternshalaHiring since September 2019236 opportunities posted45 candidates hired                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
+          <t>About the internship    Selected intern's day-to-day responsibilities include:1. Conduct legal research and analysis on various matters2. Draft legal documents, contracts, and agreements3. Assist in preparing for court hearings and trials4. Review and analyze legal documents and correspondence5. Communicate with clients, attorneys, and other legal professionals6. Maintain and organize legal files and documentation7. Provide support to the legal team as neededAny other cross-functional team support if requiredSkill(s) requiredEnglish Proficiency (Spoken)English Proficiency (Written)MS-OfficeMS-WordEarn certifications in these skillsLearn Business CommunicationLearn MS-ExcelWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 18th Jul'25 and 22nd Aug'25                                    3. are available for duration of 6 months                                    4. have relevant skills and interests                    Other requirements                    This role is not open to freshers; we require candidates with relevant experience.                                    The stipend will be based on the candidate’s skills and prior experience.                Number of openings        2                        About Movi Ecoserve Private Limited                        Movi Ecoserve works in sustainable technologies. We work majorly with the government and municipalities in pan India.     Activity on InternshalaHiring since February 202261 opportunities posted3 candidates hired                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1066,24 +1066,24 @@
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:22</t>
+          <t>2025-07-20 10:41:03</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/human-resources-hr-internship-in-jaipur-at-softsensorai1752833768</t>
+          <t>https://internshala.com/internship/detail/law-legal-internship-in-mumbai-at-movi-ecoserve-private-limited1752834353</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Finance Equity Analyst</t>
+          <t>Project Management</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>About the work from home job/internship    Are you a finance-savvy individual eager to dive into the world of equity analysis? Look no further! Savvy Merit is seeking a talented finance equity analyst intern to join our dynamic team. As an intern, you will have the opportunity to gain hands-on experience in financial analysis and market research while working closely with seasoned professionals in the industry. Selected intern's day-to-day responsibilities include:1. Conduct in-depth research and analysis on equity investments to identify potential opportunities for growth.2. Assist in the preparation of financial models and reports to support investment decisions.3. Monitor and evaluate market trends, economic developments, and company performance to make informed recommendations.4. Collaborate with team members to assess risk factors and develop strategies to mitigate potential risks.5. Present findings and recommendations to senior management and contribute to investment discussions.6. Develop a strong understanding of financial markets, investment strategies, and valuation techniques.7. Stay updated on industry news and regulations to ensure compliance with relevant guidelines.If you are passionate about finance and eager to learn from industry experts, this internship is the perfect opportunity for you to kickstart your career in equity analysis. Join us at Savvy Merit and take your first step towards a successful future in finance!Skill(s) requiredFinancial literacyEarn certifications in these skillsLearn Stocks and TradingLearn Business CommunicationLearn Business AnalyticsLearn Financial modeling valuationLearn Personal FinanceWho can applyOnly those candidates can apply who:                1. are available for the work from home job/internship                                    2. can start the work from home job/internship between 18th Jul'25 and 22nd Aug'25                                    3. are available for duration of 1 month                                    4. have relevant skills and interests                    * Women wanting to start/restart their career can also apply.PerksCertificate Letter of recommendation Flexible work hoursNumber of openings        20                        About Savvy Merit                Website         Savvy Merit is a forward-thinking educational company committed to empowering individuals with the knowledge, tools, and strategies needed to thrive in the world of finance and the stock market. Our mission is to simplify complex financial concepts and make investing accessible to everyone, from curious beginners to aspiring market professionals. We offer high-quality education through structured courses, live mentorship, interactive workshops, and market insights. Our expert-led curriculum covers a wide range of topics, including stock market fundamentals, technical and fundamental analysis, portfolio management, and financial planning, all with a focus on real-world applications. What sets us apart is our team of experienced mentors, beginner-to-advanced learning tracks, live market training and simulations, strong community support, engaging webinars, and access to up-to-date tools and resources.    Activity on InternshalaHiring since June 202559 opportunities posted                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
+          <t>About the internship    As a Project Management intern at VerboLabs, you will have the opportunity to work in a dynamic and fast-paced environment where your skills in Interpersonal communication, Effective Communication, and Time Management will be put to the test. Your role will involve collaborating with team members, clients, and vendors to ensure projects are completed successfully and on time. Key responsibilities:1. Assist in creating project plans and timelines2. Communicate project updates and progress to all stakeholders3. Coordinate with team members to delegate tasks and ensure deadlines are met4. Conduct research and analysis to support project objectives5. Assist in identifying potential risks and developing mitigation strategies6. Participate in meetings and provide input on project strategy and direction7. Maintain project documentation and ensure accuracy and completeness of recordsIf you are a proactive and driven individual looking to gain hands-on experience in project management, this internship is the perfect opportunity to expand your skills and make a real impact. Apply now and take the first step towards a rewarding career in project management at VerboLabs.Skill(s) requiredEffective CommunicationInterpersonal skillsTime ManagementEarn certifications in these skillsLearn Business CommunicationWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 18th Jul'25 and 22nd Aug'25                                    3. are available for duration of 3 months                                    4. are from Udaipur only                                    5. have relevant skills and interests                    * Women wanting to start/restart their career can also apply.PerksCertificate Letter of recommendation Job offerAdditional informationJob offer: On successful conversion to a permanent employee, the candidate can expect a salary of ₹ 240000 to 300000/year Number of openings        4                        About VerboLabs                LinkedIn page         VerboLabs is a leading language services company based in Bangalore, India. We are one of the top website &amp; human translation service providing agencies. Our great base of experienced native translators makes sure that every project is taken up sincerely and that the best efforts are put in to make it stand out in terms of quality.    Activity on InternshalaHiring since November 20227 opportunities posted                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1101,24 +1101,24 @@
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:22</t>
+          <t>2025-07-20 10:41:05</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/work-from-home-part-time-finance-equity-analyst-internship-at-savvy-merit1752840608</t>
+          <t>https://internshala.com/internship/detail/project-management-internship-in-udaipur-at-verbolabs1752837603</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Jewelry Design &amp; Creative Product</t>
+          <t>Human Resources (HR)</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>About the internship    Selected intern's day-to-day responsibilities include:1. Conceptualize and sketch disruptive jewelry and accessory designs that break the conventional mold.2. Create trend-forward moodboards, storyboards, and product visuals using Procreate, Canva, or Adobe tools.3. Contribute ideas for packaging, branding, and storytelling aligned with the brand vision.4. Support social media content design (optional) for styling, lookbooks, and creative direction.5. Design handmade sketches based on the concept shared and given.Skill(s) requiredAdobe IllustratorAdobe PhotoshopCanvaCLO3DDesign ThinkingMarket AnalysisProcreateRhinoSketchingEarn certifications in these skillsLearn Adobe PhotoshopLearn AutoCADLearn Autodesk Fusion 360Who can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 14th Jul'25 and 18th Aug'25                                    3. are available for duration of 3 months                                    4. are from Thane, Mumbai only                                    5. have relevant skills and interests                    * Women wanting to start/restart their career can also apply.Other requirements                    1. Candidates currently pursuing or recently completed a course in fashion design, accessory design, jewelry design, or product design.                                    2. Must be from Mumbai or Thane only.                                    3. Must be available for office hours.                                    4. Must have a strong interest in working on bold, creative, and unconventional concepts.                                    5. Women wanting to start/restart their careers are encouraged to apply.                PerksCertificate Letter of recommendation Flexible work hours Informal dress code 5 days a week Free snacks &amp; beveragesAdditional informationStipend Structure:Fixed pay: ₹ 3,000 - 7,000 /month                    Incentive pay: ₹ 1,000 - 5,000 /month                     Number of openings        2                        About Magic Touch                        Magic Touch has been a benchmark for design, craftsmanship, quality, and price. As India's leading manufacturer and retailer of real diamond &amp; jewelry, we offer a huge range of exclusive designs and a wide-ranging collection. Whether you are looking for everyday wear, occasion wear, or gifting, Magic Touch is your one-stop jewelry shopping destination for the best in quality, design, and price!    Activity on InternshalaHiring since May 202110 opportunities posted1 candidate hired                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
+          <t>About the internship    Position: HR InternLocation: Jaipur (Onsite)Shift Timing: Day Shift (10:00 AM to 7:00 PM)Stipend:    15,000 per monthAbout the Role:We are looking for a motivated and enthusiastic HR Intern to join our team at our Jaipur office. This is a great opportunity for individuals who are passionate about building a career in human resources and wish to gain hands-on experience in a professional setting.Key Responsibilities:Assist in recruitment processes, including sourcing, screening, and scheduling interviews.Maintain and update employee records and HR databases.Support onboarding and orientation processes for new hires.Help in organizing employee engagement activities and events.Provide support for daily HR operations and administrative tasks.Handle documentation and assist in policy compliance.Requirements:Pursuing or recently completed a degree in Human Resources, Business Administration, or a related field.Strong communication and interpersonal skills.Proficiency in MS Office (Word, Excel, PowerPoint).Ability to multitask and prioritize tasks efficiently.Positive attitude and eagerness to learn.Skill(s) requiredEnglish Proficiency (Spoken)English Proficiency (Written)MS-ExcelMS-WordRecruitmentEarn certifications in these skillsLearn Business CommunicationLearn MS-ExcelLearn about RecruitmentWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 18th Jul'25 and 22nd Aug'25                                    3. are available for duration of 4 months                                    4. are from Jaipur only                                    5. have relevant skills and interests                    PerksCertificate Letter of recommendation Flexible work hours 5 days a weekNumber of openings        1                        About Softsensor.ai                Website         Softsensor.ai is a USA and India-based corporation focused on delivering outcomes to clients using data. Our expertise lies in a collection of people, methods, and accelerators to rapidly deploy solutions for our clients. Our principals have significant experience with leading global consulting firms &amp; corporations and delivering large-scale solutions. We are focused on data science and analytics for improving the process and organizational performance. We are working on cutting-edge data science technologies like NLP, CNN, and RNN and applying them in the business context.    Activity on InternshalaHiring since September 2019236 opportunities posted45 candidates hired                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1136,24 +1136,24 @@
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:23</t>
+          <t>2025-07-20 10:41:05</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/jewelry-design-creative-product-internship-in-multiple-locations-at-magic-touch1752667067</t>
+          <t>https://internshala.com/internship/detail/human-resources-hr-internship-in-jaipur-at-softsensorai1752833768</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>UI/UX Design</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>About the work from home job/internship    Selected intern's day-to-day responsibilities include: 1. Create and schedule engaging social media posts to increase awareness and engagement2. Assist in the development and execution of email marketing campaigns to reach our target audience3. Utilize MS Office and MS Excel to analyze marketing data and trends4. Collaborate with the team to brainstorm and implement innovative marketing strategies5. Maintain and update our online presence on various platforms6. Utilize your proficiency in spoken Hindi and English to communicate effectively with our diverse audience7. Develop written content for various marketing materials to convey our message and find donors for the campaign effectivelySkill(s) requiredDigital MarketingEmail MarketingEnglish Proficiency (Spoken)English Proficiency (Written)Hindi Proficiency (Spoken)MS-ExcelMS-OfficeSocial Media MarketingEarn certifications in these skillsLearn Email MarketingLearn Business CommunicationLearn Facebook MarketingLearn Google AdWordsLearn MS-ExcelLearn Search Engine MarketingLearn SEOLearn Social Media MarketingWho can applyOnly those candidates can apply who:                1. are available for the work from home job/internship                                    2. can start the work from home job/internship between 18th Jul'25 and 22nd Aug'25                                    3. are available for duration of 2 weeks                                    4. have relevant skills and interests                    PerksCertificate Letter of recommendation Flexible work hours 5 days a weekNumber of openings        6                        About Rural Development Society                        Rural Development Society (RDS) is a dedicated non-profit organization passionately committed to the holistic development of rural communities. Specializing in children's welfare and social empowerment, we collaborate seamlessly with numerous NGOs, fostering a united front for positive change. Together, we strive to create a brighter future, one where every child has the opportunity to thrive and every community can flourish. Join us in our mission to uplift lives and build a more inclusive society.    Activity on InternshalaHiring since November 2023272 opportunities posted9779 candidates hired                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
+          <t>About the internship    As a UI/UX Design intern, you will have the opportunity to work on cutting-edge projects and gain hands-on experience in the field. Your creativity and skills in Wireframing, UI and UX Design, Figma, Sketch, and Adobe Illustrator will be put to the test as you collaborate with our team to create user-friendly interfaces for our digital platforms.Key Responsibilities:1. Collaborate with the product officer to create wireframes and prototypes for new features and enhancements.2. Conduct user research and testing to gather insights and feedback for design improvements.3. Work closely with developers to ensure designs are implemented accurately and efficiently.4. Create visually appealing and intuitive designs that enhance the overall user experience.5. Stay up-to-date with the latest design trends and technologies to continually improve our products.6. Assist in the creation of design assets and style guides to maintain brand consistency.7. Participate in design reviews and provide constructive feedback to help refine design concepts. If you are a motivated and creative individual looking to jumpstart your career in UI/UX design, we want to hear from you! Join us and be part of a dynamic team that is shaping the future.Skill(s) requiredAdobe IllustratorFigmaSketchUI &amp; UX DesignWireframingEarn certifications in these skillsLearn FigmaLearn Rapid PrototypingLearn UI &amp; UX DesignLearn WireframingWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 18th Jul'25 and 22nd Aug'25                                    3. are available for duration of 2 months                                    4. are from Coimbatore only                                    5. have relevant skills and interests                    PerksCertificate Letter of recommendation Flexible work hours Informal dress codeNumber of openings        1                        About HiFresh Agro Private Limited                        HiFresh Agro Private Limited is a startup focused on producing protein-rich food such as mushrooms and Spirulina, with strategic plans to expand into the export business of agricultural products such as millets, coir, and other agricultural produce where there is a demand.    Activity on InternshalaHiring since June 202416 opportunities posted8 candidates hired                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1163,7 +1163,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Web Development Internship</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
@@ -1171,24 +1171,24 @@
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:23</t>
+          <t>2025-07-20 10:41:06</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/work-from-home-marketing-internship-at-rural-development-society1752840612</t>
+          <t>https://internshala.com/internship/detail/ui-ux-design-internship-in-coimbatore-at-hifresh-agro-private-limited1752838475</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Next.js Development</t>
+          <t>Search Engine Optimization (SEO)</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>About the work from home job/internship    Selected intern's day-to-day responsibilities include: 1. Convert Framer prototypes/designs into hard-coded front-end pages using Next.js, HTML, and CSS2. Ensure responsive design, cross-browser compatibility, and performance3. Collaborate with designers and developers to maintain design consistencyMaintain clean, well-documented code4. Optimize components for performance and scalabilitySkill(s) requiredCSSFramerHTMLNext.jsEarn certifications in these skillsLearn CSSLearn HTMLLearn Web DevelopmentLearn Data Structures &amp; AlgorithmsLearn Git &amp; GithubLearn NodejsLearn Business CommunicationWho can applyOnly those candidates can apply who:                1. are available for the work from home job/internship                                    2. can start the work from home job/internship between 18th Jul'25 and 22nd Aug'25                                    3. are available for duration of 2 months                                    4. have relevant skills and interests                    Other requirements                    1. Basic understanding of Next.js, React, HTML, and CSS                                    2. Ability to accurately translate visual designs into code                                    3. Familiarity with responsive and adaptive design principles                                    4. Attention to detail and a sense of design aesthetics                                    5. Eagerness to learn and take feedback constructively                PerksCertificate Letter of recommendation Flexible work hoursNumber of openings        2                        About Aadi Foundation                        Aadi Foundation started in 2021, is a non-profit organization committed to bringing the best educational resources to the under-served tribal communities of Delhi, Dehradun, etc., in India. We also distribute food items in poverty-stricken areas and always stress activities and strategies that cover the whole cycle of what is required for providing quality education and food to an individual child in a structured manner. Our mission is to build a platform for vulnerable and oppressed children, living in poverty, thus empowering them with well-equipped education and gaining knowledge to alleviate poverty.    Activity on InternshalaHiring since July 2022208 opportunities posted1002 candidates hired                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
+          <t>About the internship    Selected intern's day-to-day responsibilities include: 1. Assist in creating backlinks through methods like citations, profile creation, classified ads, and blog commenting2. Conduct keyword research using SEO tools to identify high-performing search terms3. Perform competitor analysis to understand SEO strategies, backlink profiles, and keyword gaps4. Support in technical SEO audits and reporting5. Write and optimize meta titles and descriptions for improved CTR and SERP rankings6. Analyze website traffic and user behavior using tools like Google Analytics and Search Console7. Help in content optimization for blog posts, landing pages, and service pages based on SEO best practices8. Monitor and report daily/weekly keyword rankings and SEO performance metrics9. Research and list relevant directories and platforms for off-page SEO10. Stay updated with the latest SEO trends, Google algorithm updates, and industry tools11. Collaborate with the team to brainstorm and execute link-building strategies12. Support in on-page SEO elements such as header tags, image optimization, and internal linkingSkill(s) requiredComputer skillsEnglish Proficiency (Written)Google Keyword PlannerMicrosoft PowerAppsSearch Engine Optimization (SEO)Earn certifications in these skillsLearn Business CommunicationLearn MS-ExcelLearn SEOWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 18th Jul'25 and 22nd Aug'25                                    3. are available for duration of 6 months                                    4. are from Jaipur only                                    5. have relevant skills and interests                    * Women wanting to start/restart their career can also apply.Other requirements                    1. Strong interest in digital marketing and content strategy                                    2. Ability to conduct online research and summarize findings clearly                                    3. Comfortable using spreadsheets (Google Sheets/Excel) for tracking SEO data                                    4. Eagerness to learn and stay updated on SEO trends and Google algorithm changes                                    5. Ability to follow instructions and meet deadlines                                    6. Self-motivated, proactive, and detail-oriented mindset                                    Bonus: Experience with WordPress or other CMS platforms                                    Bonus: Familiarity with ChatGPT or other AI tools for content ideation and SEO research                PerksCertificate Letter of recommendation Informal dress codeNumber of openings        5                        About Jaipur SEO Company                Website         We are a bunch of relentless tech nerds aiming to grow ahead of digital trends. Having served businesses in 15+ domain verticals and 40+ business niches serving a wide array of audiences, we have delivered top organic positions and paid leverages through result-focused search marketing and digital branding services. We have been a service trusted by local businesses and inventive brands. A 95% target-achievement rate and 80% business retention figures define the crux of it.    Activity on InternshalaHiring since September 202313 opportunities posted4 candidates hired                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1198,7 +1198,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Web Development Internship</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E22" t="inlineStr"/>
@@ -1206,24 +1206,24 @@
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:24</t>
+          <t>2025-07-20 10:41:07</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/work-from-home-nextjs-development-internship-at-aadi-foundation1752839954</t>
+          <t>https://internshala.com/internship/detail/search-engine-optimization-seo-internship-in-jaipur-at-jaipur-seo-company1752846589</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Company Secretary (CS)</t>
+          <t>Flutter Development</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>About the internship    Selected intern's day-to-day responsibilities include:1. Assisting with MCA-related tasks, including company incorporation, amendment of AOA/MOA, charge filing, and annual return and accounts filing2. Performing accounting work using accounting software3. Liaisoning with clients for documentation and compliance coordinationSkill(s) requiredAccountingEnglish Proficiency (Spoken)English Proficiency (Written)MS-ExcelMS-OfficeEarn certifications in these skillsLearn Business CommunicationLearn MS-ExcelLearn TallyWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 18th Jul'25 and 22nd Aug'25                                    3. are available for duration of 6 months                                    4. have relevant skills and interests                    Number of openings        4                        About KNSG &amp; CO LLP                        The CA firm has 10 years of experience and works on all kinds of audit-related work, taxation work (income tax, GST, etc.), banking-related work like stock audits, and MCA-related work. We are offering the opportunity to work directly with CA Naman Singla (ex-KPMG) and CA Ripika Gupta (ex-ICICI) as a risk analyst.    Activity on InternshalaHiring since January 202316 opportunities posted1 candidate hired                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
+          <t>About the internship    Selected intern's day-to-day responsibilities include: 1. Develop secure, scalable, and high-performance mobile applications using modern frameworks and best practices2. Collaborate with backend developers and designers to integrate APIs and deliver seamless user experiences3. Support and mentor teammates by reviewing code, sharing knowledge, and assisting with mobile development challengesSkill(s) requiredDartFlutterEarn certifications in these skillsLearn Andoid App DevelopementLearn Android App DevelopmentLearn Git &amp; GithubWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 19th Jul'25 and 23rd Aug'25                                    3. are available for duration of 6 months                                    4. are from Ahmedabad only                                    5. have relevant skills and interests                    * Women wanting to start/restart their career can also apply.Other requirements                    1. Candidates currently pursuing a degree in computer science, information technology, or related fields are preferred                                    2. Must possess a strong willingness to learn and adapt in a fast-paced environment                                    3. Basic understanding of programming concepts, mobile app development (Flutter/React Native/Android/iOS), and UI/UX principles is a plus                                    4. Good communication skills and the ability to work collaboratively in a team                                    5. A proactive attitude with a problem-solving mindset is highly desirable                                    6. Eagerness to take on challenges and contribute to real-world projects                PerksCertificate Letter of recommendation Informal dress code Free snacks &amp; beveragesAdditional informationStipend Structure:Fixed pay: ₹ 4,000 - 7,000 /month                    Incentive pay: ₹ 1,000 - 3,000 /month                     Number of openings        3                        About Arhant Solutions                Website         Arhant Solutions is an IT services company based in Ahmedabad. We offer expert solutions tailored to meet your business needs with cutting-edge technology and dedicated support.    Activity on InternshalaHiring since December 20245 opportunities posted                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1241,24 +1241,24 @@
       <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:25</t>
+          <t>2025-07-20 10:41:08</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/company-secretary-cs-internship-in-delhi-at-knsg-co-llp1752824459</t>
+          <t>https://internshala.com/internship/detail/flutter-development-internship-in-ahmedabad-at-arhant-solutions1752899652</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Graphic Designer (Pharmaceuticals, Nutraceuticals, And Cosmetics)</t>
+          <t>Content Marketing</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>About the internship    As a graphic designer intern at ACTBLENDX INGREDIENTS PRIVATE LIMITED, you will have the opportunity to work on exciting projects and gain valuable hands-on experience in the field. We are looking for a talented individual who is proficient in Adobe Creative Suite, typography, layout design, UI &amp; UX design, logo design, color theory, digital design, and effective communication skills.Selected intern's day-to-day responsibilities include: 1. Collaborate with the design team to create visually appealing graphics for various marketing materials.2. Assist in the development of brand identity assets, including logos, color schemes, and typography.3. Design user-friendly interfaces for our website and digital platforms, focusing on enhancing the user experience.4. Utilize your knowledge of color theory to create eye-catching designs that resonate with our target audience.5. Ensure consistency in design across all platforms and materials, maintaining a cohesive brand image.6. Communicate effectively with team members to understand project requirements and deliver high-quality designs on time.7. Stay updated on industry trends and best practices to continuously improve your design skills and contribute fresh ideas to the team.Skill(s) requiredAdobe Creative SuiteColor TheoryDigital DesignEffective CommunicationLayout DesignLogo DesignTypographyUI &amp; UX DesignEarn certifications in these skillsLearn Adobe After EffectsLearn Colour Theory for DesignersLearn Adobe PhotoshopLearn Adobe Premiere ProLearn FigmaLearn Rapid PrototypingLearn UI &amp; UX DesignLearn WireframingWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 18th Jul'25 and 22nd Aug'25                                    3. are available for duration of 3 months                                    4. have relevant skills and interests                    * Women wanting to start/restart their career can also apply.Other requirements                    1. Previous experience in healthcare, medical, or wellness writing                                    2. Knowledge of regulatory compliance in health/pharma content                                    3. Understanding of audience targeting and digital content best practices                PerksCertificate Letter of recommendation 5 days a weekNumber of openings        4                        About ACTBLENDX INGREDIENTS PRIVTE LIMITED                Website         ActBlendex Ingredients is a research-driven organization, empowering wellbeing through next generation nutritional innovation through supplying and manufacturing API's and ingredients for Pharmaceuticals, Nutraceuticals, Bakery, Dairy, Spices and Ani. With increasing education and awareness of preventive health, encouraging peoples to think differently about health and wellness, and creating momentum for nutraceuticals. It's our constant endeavor to research &amp; development for products and technologies to provide solutions for optimum health and healthy lifestyle.We at ActBlendex are focused on human wellness through supplements and functional foods. We have developed an entire product pipeline &amp; technologies to conquer the unmet health and market need using advanced nanotechnology and biotechnological process.    Activity on InternshalaHiring since November 201822 opportunities posted                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
+          <t>About the internship    Selected intern's day-to-day responsibilities include:1. Research &amp; trends: Conduct research on travel trends, destinations, and audience preferences to produce relevant and impactful content.2. Product content enhancement: Add engaging and persuasive content for our travel products, ensuring descriptions are compelling, informative, and aligned with our brand voice and marketing objectives.3. Content marketing: Assist in planning and implementing content marketing campaigns across digital platforms.4. SEO &amp; analytics: Learn and apply SEO best practices; monitor content performance and provide insights for optimization.5. Collaboration: Work closely with marketing, design, and product teams to ensure cohesive campaigns and messaging.6. Editing &amp; proofreading: Review and refine content to ensure accuracy, clarity, and consistency.Skill(s) requiredCreative WritingEffective CommunicationGoogle AdWordsMarketing Campaigns Search Engine Optimization (SEO)Earn certifications in these skillsLearn Creative WritingLearn Google AdWordsLearn SEOWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 18th Jul'25 and 22nd Aug'25                                    3. are available for duration of 6 months                                    4. are from Jaipur only                                    5. have relevant skills and interests                    Other requirements                    1. Creative thinker with a passion for travel and digital storytelling.                                    2. Strong writing and communication skills in English.                                    3. Understanding of social media, digital marketing, and basic SEO principles.                                    4. Ability to research, analyze trends, and adapt content accordingly.                                    5. Team player with strong collaboration and organizational skills.                                    6. Currently pursuing or recently graduated in marketing, mass communication, Journalism, English, or related fields.                                    7. Familiarity with Google Workspace (Docs, Sheets) and basic knowledge of SEO is preferred.                                    8. Portfolio or writing samples showcasing your skills are a plus (optional but recommended).                PerksCertificateNumber of openings        1                        About Travel Lykke Private Limited                Website         We are a travel brand curating unique, experiential &amp; sustainable holidays for you. Our trips are not limited to usual travel arrangements. We design unique, immersive experiences that make their mark in your heart. We also believe in sustainable tourism. We try to make our trips as environmentally friendly as possible and engage local communities in the destinations. Other than the usual blah blah blah, we are a bunch of youngsters, insanely passionate about travel. We think of you as our future friends and not just customers.    Activity on InternshalaHiring since February 202527 opportunities posted13 candidates hired                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1276,24 +1276,24 @@
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:25</t>
+          <t>2025-07-20 10:41:08</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/graphic-designer-pharmaceuticals-nutraceuticals-and-cosmetics-internship-in-gurgaon-at-actblendx-ingredients-privte-limited1752838781</t>
+          <t>https://internshala.com/internship/detail/content-marketing-internship-in-jaipur-at-travel-lykke-private-limited1752844515</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Human Resources (HR)</t>
+          <t>Business Development (Sales)</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>About the internship    Selected intern's day-to-day responsibilities include: 1. Manage the recruitment process from sourcing candidates to conducting interviews and making offers.2. Screen resumes and conduct initial phone screenings to ensure candidates meet job requirements.3. Handle payroll processing and ensure accuracy in payroll calculations.4. Conduct regular audits to ensure compliance with company policies and legal requirements.5. Develop and implement HR policies and procedures to streamline processes and improve efficiency.6. Coordinate training and development programs for employees to enhance their skills and knowledge.7. Provide guidance and support to employees on HR-related matters and foster a positive and inclusive work environment.Skill(s) requiredEffective CommunicationEnglish Proficiency (Spoken)English Proficiency (Written)Google WorkspaceInterpersonal skillsRecruitmentResume screeningEarn certifications in these skillsLearn Business CommunicationLearn MS-ExcelLearn about RecruitmentWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 18th Jul'25 and 22nd Aug'25                                    3. are available for duration of 4 months                                    4. are from Delhi, Gurgaon, Greater Noida, Noida, Greater Noida West only                                    5. have relevant skills and interests                    * Women wanting to start/restart their career can also apply.Other requirements                    1. Strong communication skills (verbal and written) in English and Hindi.                                    2. Available to work full-time in-office for a minimum of 4 months.                PerksCertificate Letter of recommendation Informal dress code 5 days a week Free snacks &amp; beveragesNumber of openings        4                        About Swing Saga                Website         At Swing Saga, our range of products is curated to provide a one-stop shop for reasonably priced and unique home decor. Whether your preference is bohemian, chic, antique, or modern, we have the right thing for you. At the core of our philosophy is the combination of creativity and innovation to give you products that look beautiful and can stand the test of time, too. Whether it's our outdoor LED planters or handcrafted bed swings, we use high-quality materials to ensure a sumptuous yet sturdy design. We wish to give you the best of both worlds because your home deserves nothing less. Our women-led venture is an effort to bring you great ecological products at affordable prices, backed by great customer service. Every day, we strive to create long, trustworthy relationships. As your home evolves with you, we promise we'll continue to bring you exquisite decor that you will love. We hope you find a little bit of yourself in our humble store.    Activity on InternshalaHiring since April 202346 opportunities posted1 candidate hired                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
+          <t>About the internship    Selected intern's day-to-day responsibilities:1. Generate leads and prospect potential clients2. Provide support to the sales team in daily operations3. Conduct market and competitor research to identify opportunities4. Interact with customers to understand their needs and build relationships5. Gain a thorough understanding of the product and its value propositionSkill(s) requiredE-commerceEnglish Proficiency (Spoken)English Proficiency (Written)MS-ExcelEarn certifications in these skillsLearn Business CommunicationLearn MS-ExcelLearn Digital MarketingLearn Business AnalyticsWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 19th Jul'25 and 23rd Aug'25                                    3. are available for duration of 6 months                                    4. are from Palghar, Thane, Navi Mumbai, Mumbai only                                    5. have relevant skills and interests                    PerksCertificate Letter of recommendation Informal dress code Job offerAdditional informationJob offer: On successful conversion to a permanent employee, the candidate can expect a salary of ₹ 240000 to 300000/year Number of openings        2                        About Vamaship                Website         Vamaship is a tech-driven logistics aggregator that empowers e-commerce sellers across India. By partnering with leading courier services like BlueDart and Delhivery, Vamaship streamlines shipping through real-time tracking, delivery &amp; returns management, COD management, and timely communication at critical milestones. As an intern, you'll gain hands-on experience in a dynamic environment, learning about cutting-edge supply chain technology while helping create seamless shipping solutions for growing online businesses.    Activity on InternshalaHiring since July 20253 opportunities posted                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1311,12 +1311,12 @@
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:26</t>
+          <t>2025-07-20 10:41:09</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/human-resources-hr-internship-in-multiple-locations-at-swing-saga1752835821</t>
+          <t>https://internshala.com/internship/detail/business-development-sales-internship-in-multiple-locations-at-vamaship1752924797</t>
         </is>
       </c>
     </row>
@@ -1346,7 +1346,7 @@
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:27</t>
+          <t>2025-07-20 10:41:09</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -1358,12 +1358,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Video Editor/Maker (Pharmaceuticals, Nutraceuticals, And Cosmetics)</t>
+          <t>Front End Development</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>About the internship    As a Video Editing/Making intern at ACTBLENDX INGREDIENTS PRIVATE LIMITED, you will have the exciting opportunity to showcase your skills in Adobe Premiere Pro, After Effects, Canva, Final Cut Pro, Photoshop, Illustrator, and motion graphics. You will be an integral part of our creative team, bringing our brand to life through visually compelling videos. Selected intern's day-to-day responsibilities include: 1. Collaborate with the marketing team to create engaging video content for social media, website, and other platforms.2. Edit and enhance raw footage to produce high-quality videos that align with the company's brand and message.3. Incorporate motion graphics and animation to elevate the visual appeal of our videos.4. Brainstorm and pitch creative ideas for video projects that will resonate with our target audience.5. Maintain a keen eye for detail, ensuring all videos are polished and error-free before publication.6. Stay up-to-date on industry trends and best practices to continually improve your video editing skills.7. Assist with other creative projects as needed to support the overall marketing efforts of the company. This internship will provide you with hands-on experience in video production and editing, valuable skills that will set you up for success in the fast-paced world of digital marketing. Join us in bringing our brand to the next level through the power of visual storytelling.Skill(s) requiredAdobe After EffectsAdobe IllustratorAdobe PhotoshopAdobe Premiere ProCanvaFinal Cut ProMotion GraphicsPerplexityVideo EditingVideo MakingEarn certifications in these skillsLearn Adobe After EffectsLearn Adobe PhotoshopLearn Adobe Premiere ProLearn Video EditingWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 18th Jul'25 and 22nd Aug'25                                    3. are available for duration of 3 months                                    4. have relevant skills and interests                    * Women wanting to start/restart their career can also apply.Other requirements                    1. Previous experience in healthcare, medical, or wellness.                                    2. Knowledge of regulatory compliance in health/pharma content and video editing/making.                                    3. Understanding of audience targeting and digital content best practices                                    4. Opportunity for a full-time position based on performance, creativity, and initiative                PerksCertificate Letter of recommendation 5 days a weekNumber of openings        4                        About ACTBLENDX INGREDIENTS PRIVTE LIMITED                Website         ActBlendex Ingredients is a research-driven organization, empowering wellbeing through next generation nutritional innovation through supplying and manufacturing API's and ingredients for Pharmaceuticals, Nutraceuticals, Bakery, Dairy, Spices and Ani. With increasing education and awareness of preventive health, encouraging peoples to think differently about health and wellness, and creating momentum for nutraceuticals. It's our constant endeavor to research &amp; development for products and technologies to provide solutions for optimum health and healthy lifestyle.We at ActBlendex are focused on human wellness through supplements and functional foods. We have developed an entire product pipeline &amp; technologies to conquer the unmet health and market need using advanced nanotechnology and biotechnological process.    Activity on InternshalaHiring since November 201822 opportunities posted                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
+          <t>About the internship    Selected intern's day-to-day responsibilities include: 1.Ensuring the technical feasibility of UI/UX designs and optimizing applications for speed and scalability2.Debugging and resolving frontend issues and browser compatibility problems3.Developing user-facing features using HTML, CSS, JavaScript, and modern frameworks like React.js or Vue.jsSkill(s) requiredCSSHTMLJavaScriptNext.jsReactEarn certifications in these skillsLearn AngularLearn CSSLearn HTMLLearn Node.JS using JavascriptLearn Software Testing using JavascriptLearn Node.JSLearn ReactJSWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 19th Jul'25 and 23rd Aug'25                                    3. are available for duration of 6 months                                    4. are from Jaipur only                                    5. have relevant skills and interests                    PerksCertificate Letter of recommendation Job offerAdditional informationJob offer: On successful conversion to a permanent employee, the candidate can expect a salary of ₹ 300000 to 360000/year Number of openings        2                        About Gurucool                Instagram page         Gurucool is an online platform for astrology and Kundli predictions from the best astrologers in India. Users can talk to astrologers on call or live chat. They can also opt for a complete annual astrological report or post a question on astrology. Astrology questions could be on any subject, from marriage and love life to career or health.    Activity on InternshalaHiring since April 2019751 opportunities posted90 candidates hired                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1381,24 +1381,24 @@
       <c r="G27" t="inlineStr"/>
       <c r="H27" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:27</t>
+          <t>2025-07-20 10:41:10</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/video-editor-maker-pharmaceuticals-nutraceuticals-and-cosmetics-internship-in-gurgaon-at-actblendx-ingredients-privte-limited1752838409</t>
+          <t>https://internshala.com/internship/detail/front-end-development-internship-in-jaipur-at-gurucool1752902543</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Sales and Marketing</t>
+          <t>Company Secretary (CS)</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>About the internship    Selected intern's day-to-day responsibilities include: 1. Identify suitable leads using portals and online data sources2. Call leads to explain the product and schedule a demo3. Maintain the log of sales leads and status reportsSkill(s) requiredEffective CommunicationEarn certifications in these skillsLearn Business CommunicationLearn Digital MarketingLearn Business AnalyticsWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 18th Jul'25 and 22nd Aug'25                                    3. are available for duration of 3 months                                    4. are from Pune only                                    5. have relevant skills and interests                    Other requirements                    1. MBA in Sales and marketing                PerksCertificate Letter of recommendation Informal dress code Job offerAdditional informationStipend Structure:Fixed pay: ₹ 10,000 - 10,001 /month                    Incentive pay: ₹ 5,000 - 20,000 /month                     Job offer: On successful conversion to a permanent employee, the candidate can expect a salary of ₹ 200000 to 300000/year Number of openings        2                        About Quantian Technologies Private Limited                        We help small &amp; medium companies leverage the power of emerging digital technologies to enable a non-linear growth trajectory. Services include digital onboarding via high-performance and visually appealing websites, light &amp; progressive web applications, hybrid and cross-platform mobile applications, AI/ML utilities, IoT solutions, and more.     Activity on InternshalaHiring since April 202117 opportunities posted4 candidates hired                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
+          <t>About the internship    Selected intern's day-to-day responsibilities include:1. Assisting with MCA-related tasks, including company incorporation, amendment of AOA/MOA, charge filing, and annual return and accounts filing2. Performing accounting work using accounting software3. Liaisoning with clients for documentation and compliance coordinationSkill(s) requiredAccountingEnglish Proficiency (Spoken)English Proficiency (Written)MS-ExcelMS-OfficeEarn certifications in these skillsLearn Business CommunicationLearn MS-ExcelLearn TallyWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 18th Jul'25 and 22nd Aug'25                                    3. are available for duration of 6 months                                    4. have relevant skills and interests                    Number of openings        4                        About KNSG &amp; CO LLP                        The CA firm has 10 years of experience and works on all kinds of audit-related work, taxation work (income tax, GST, etc.), banking-related work like stock audits, and MCA-related work. We are offering the opportunity to work directly with CA Naman Singla (ex-KPMG) and CA Ripika Gupta (ex-ICICI) as a risk analyst.    Activity on InternshalaHiring since January 202316 opportunities posted1 candidate hired                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1416,24 +1416,24 @@
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:28</t>
+          <t>2025-07-20 10:41:11</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/sales-and-marketing-internship-in-pune-at-quantian-technologies-private-limited1752826302</t>
+          <t>https://internshala.com/internship/detail/company-secretary-cs-internship-in-delhi-at-knsg-co-llp1752824459</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Telecalling (Tamil, Telugu, English &amp; Hindi)-Female</t>
+          <t>Business Development (Sales)</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>About the work from home job/internship    Selected intern's day-to-day responsibilities include making 150+ connected calls daily, diligently following up with prospects, and ensuring effective communication to maximize conversions and project success.Skill(s) requiredEnglish Proficiency (Spoken)English Proficiency (Written)Hindi Proficiency (Spoken)Hindi Proficiency (Written)MarketingSalesTamil Proficiency (Spoken)Tamil Proficiency (Written)Telugu Proficiency (Spoken)Telugu Proficiency (Written)Earn certifications in these skillsLearn Email MarketingLearn Business CommunicationLearn Facebook MarketingLearn Google AdWordsLearn Search Engine MarketingLearn SEOLearn Social Media MarketingWho can applyOnly those candidates can apply who:                1. are available for the work from home job/internship                                    2. can start the work from home job/internship between 18th Jul'25 and 22nd Aug'25                                    3. are available for duration of 6 months                                    4. have relevant skills and interests                    * Women wanting to start/restart their career can also apply.Other requirements                    1. Fluency in Hindi, English, and regional languages (Tamil &amp; Telugu) is necessary.                                    2. Applications from female candidates are encouraged.                                    3. Access to a laptop and an Android mobile phone is required.                                    4. The ability to follow up and close leads is essential.                PerksCertificate Letter of recommendationNumber of openings        10                        About Lead Mines Media                        We're the leading and quickest-growing digital marketing agency in Mumbai. We offer SMM, web designing, lead generation, SEO, tele-calling, PR, e-commerce seller account handling, and many other online services. We're not just another aspiring digital marketing company but a company that offers many services, starting from the very basics like web page styling and web development to innovative and complex development and jobs like SEO, digital marketing, and other marketing alternatives.    Activity on InternshalaHiring since May 20211654 opportunities posted2 candidates hired                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
+          <t>About the internship    Selected intern's day-to-day responsibilities: 1. Research and identify potential colleges and institutions for program partnerships2. Approach college principals, HODs, and management to present Tutorac's offerings3. Conduct in-person or virtual meetings to pitch the Career Advancement Program4. Clearly explain program benefits and address any questions/objections from college management5. Get approvals and assist in signing MoUs and onboarding colleges6. Coordinate with Tutorac's central team for seminar scheduling and student engagement activities7. Maintain a database of colleges approached and prepare weekly progress reportsSkill(s) requiredBusiness DevelopmentClient RelationshipComputer skillsEnglish Proficiency (Spoken)English Proficiency (Written)MarketingSalesTelugu Proficiency (Spoken)Web developmentEarn certifications in these skillsLearn BootstrapLearn Business CommunicationLearn CSSLearn Email MarketingLearn Facebook MarketingLearn Google AdWordsLearn HTMLLearn MS-ExcelLearn PHPLearn Search Engine MarketingLearn SEOLearn Social Media MarketingLearn AngularJSLearn AngularLearn Node.JSLearn Node.JS using JavascriptLearn Software Testing using JavascriptLearn ReactJSWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 18th Jul'25 and 22nd Aug'25                                    3. are available for duration of 3 months                                    4. are from Hyderabad only                                    5. have relevant skills and interests                    Other requirements                    1. Demonstrate excellent communication and persuasion skills in English and regional languages                                    2. Exhibit confidence while speaking to senior decision-makers like principals or directors                                    3. Show enthusiasm for career counseling, EdTech, and student empowerment                                    4. Display willingness to travel locally for college visits                                    5. Maintain self-motivation, target orientation, and eagerness to learn                PerksCertificate Letter of recommendation Job offerAdditional informationJob offer: On successful conversion to a permanent employee, the candidate can expect a salary of ₹ 300000 to 480000/year Number of openings        4                        About Request IT Support                Website         Request IT Support is a national mid-sized consulting firm positioned between the small boutiques and the big six   big enough for great opportunities and small enough for your accomplishments to be noticed and recognized. We specialize in delivering superior-quality consulting and staffing solutions to our client partners, enabling them to compete in today's competitive and dynamic business environment.     Activity on InternshalaHiring since August 2024138 opportunities posted                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1451,24 +1451,24 @@
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:28</t>
+          <t>2025-07-20 10:41:11</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/work-from-home-telecalling-tamil-telugu-english-hindi-female-internship-at-lead-mines-media1752828523</t>
+          <t>https://internshala.com/internship/detail/business-development-sales-internship-in-hyderabad-at-request-it-support1752898271</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Business Development (Sales)</t>
+          <t>Social Media Assistance</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>About the internship    Selected intern's day-to-day responsibilities include:1.  Handle *inbound &amp; outbound calls* to engage potential clients.    2.  Guide candidates through *technical counseling* for training programs.    3.  Provide information on IT courses and career paths.    4.  Build and maintain strong client relationships.    5.  Maintain accurate records of client interactions and follow-ups.    6.  Work closely with the sales and training teams for seamless operations.     Requirements:  1. MBA pass-out (Freshers can apply).    2. Strong *communication &amp; persuasion skills*.    3. Ability to manage client queries professionally.    4. Self-motivated and results-driven mindset.    Skill(s) requiredClient Relationship Management (CRM)Cold CallingEnglish Proficiency (Spoken)English Proficiency (Written)Inside SalesMS-ExcelEarn certifications in these skillsLearn Business CommunicationLearn MS-ExcelLearn Digital MarketingLearn Business AnalyticsWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 18th Jul'25 and 22nd Aug'25                                    3. are available for duration of 3 months                                    4. are from Bangalore only                                    5. have relevant skills and interests                    * Women wanting to start/restart their career can also apply.Other requirements                    MBA Marketing looking for the Internship                                    Women candidates need to restart your career can also apply                PerksCertificate Job offerAdditional informationStipend Structure:Fixed pay: ₹ 5,000 - 8,000 /month                    Incentive pay: ₹ 5,000 - 10,000 /month                     Job offer: On successful conversion to a permanent employee, the candidate can expect a salary of ₹ 200000 to 400000/year Number of openings        5                        About RADICAL TECHNOLOGIES                Website         Radical Technologies has been a recognized leader in training administrative and software development courses since 1995, empowering IT professionals with a competitive edge to tap into job opportunities in the IT sector. Dedicated to simplifying technology trends, Radical Technologies excels with its robust R&amp;D division.    Activity on InternshalaHiring since May 20189 opportunities posted                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
+          <t>About the internship    Selected intern's day-to-day responsibilities include: 1. Post daily stories to engage the audience2. Publish content on the grid every day3. Brainstorm and create fresh, engaging content4. Edit videos to enhance quality and impactSkill(s) requiredCanvaEffective CommunicationVideo MakingEarn certifications in these skillsLearn Adobe Premiere ProLearn Video EditingLearn Creative WritingLearn Business CommunicationLearn Digital MarketingLearn Business AnalyticsWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 19th Jul'25 and 23rd Aug'25                                    3. are available for duration of 3 months                                    4. are from Mumbai only                                    5. have relevant skills and interests                    Other requirements                    1. Someone who loves posting on social media                                    2. Someone who understands how social media works and audience preferences                                    3. Someone who understands Instagram and how to work the algorithm                PerksCertificate Letter of recommendationNumber of openings        1                        About The Mould Story                Website         We are a D2C brand that sells silicone molds to artists and creators. Our e-commerce website is www.themouldstory.com. Our goal is to help our customers grow their businesses by creating wonderful products that appeal to a range of customers. Our company is only 2 years old but leads the way in the manufacture and supply of quality molds for resin art, and our range is soon going to expand to other mediums as well.     Activity on InternshalaHiring since August 202324 opportunities posted3 candidates hired                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1486,24 +1486,24 @@
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:29</t>
+          <t>2025-07-20 10:41:12</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/business-development-sales-internship-in-bangalore-at-radical-technologies1752828696</t>
+          <t>https://internshala.com/internship/detail/social-media-assistance-internship-in-mumbai-at-the-mould-story1752925393</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Customer Support Specialist</t>
+          <t>UI/UX Design</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>About the internship    Customer support specialist intern at DoubleTick requires a unique blend of technical expertise, communication skills, and customer service abilities. Moreover, you must have an ownership mindset, a sense of pride in solving complex problems for our customers, owning up to the customer problems as if they were your own, and bringing a smile to our customer's faces at the end of the day. Selected intern's day-to-day responsibilities include:1. Strong understanding of SaaS products- its features, functionalities, and integrations ecosystem.2. Proficiency in troubleshooting technical issues related to DoubleTick, including but not limited to bugs, errors, and user interface problems.3. Excellent communication skills, both written and verbal, to interact effectively with customers. This includes active listening, empathy, and clarity in explanations.4. Patience and the ability to remain calm and composed, especially when dealing with frustrated or upset customers.  5. Strong problem-solving skills and analytical ability to address customer concerns and find appropriate solutions promptly.  6. Continuous hunger to learn and stay updated on the product's latest features, updates, and enhancements.7. Ability to articulate complex automation and workflow concepts in a simple and understandable manner to customers of varying technical backgrounds.8. Ability to collaborate with cross-functional teams such as product development, sales, and marketing to provide comprehensive support to customers.9. Sharing insights and feedback gathered from customer interactions to contribute to product improvement and enhancement.10. Ability to manage multiple customer inquiries simultaneously while ensuring timely responses and resolutions.11. Prioritizing tasks based on urgency and impact on customer satisfaction.12. Being adaptable to evolving processes, technologies, and customer needs in a fast-paced SaaS environment.13. Resilience in handling high-pressure situations and maintaining a positive attitude even during challenging times.14. Attention to detail in documenting customer issues, resolutions, and any follow-up actions taken.15. Conducting testing and replication of reported issues to verify resolutions and prevent recurrence.16. Proficiency in utilizing available tools to achieve high efficiency and timely responses to customers.Note - This internship does not come with a guaranteed PPO; conversion to a full-time role will be based on performance during the internship.Skill(s) requiredEffective CommunicationProblem SolvingTechnical SupportTroubleshootingEarn certifications in these skillsLearn Business CommunicationWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 18th Jul'25 and 22nd Aug'25                                    3. are available for duration of 6 months                                    4. are from Mumbai only                                    5. have relevant skills and interests                    Other requirements                    -B.Tech / B.E. (Any specialization, especially Computer Science, IT, Electronics)                                    -B.Sc / M.Sc (Computer Science, IT, or related fields)                                    -BCA / MCA                                    -BBA / MBA (preferably with a specialization in Marketing, IT, or Operations)                                    -B.Com / M.Com (for candidates with strong communication and customer-facing skills)                PerksCertificate Letter of recommendation Flexible work hours Informal dress codeNumber of openings        10                        About Apport Software Solutions Private Limited                        Apport Software Solutions Private Limited is a dynamic and innovative SAAS-based product company offering conversational commerce and empowering global brands with scalable personal commerce and relationship-led sales on WhatsApp.  QuickSell is a sales acceleration commerce suite started in 2017 with the vision to empower businesses to translate conversations into conversions on customer-first channels like WhatsApp through assisted personal commerce. For more details, check out our website: https://quicksell.co/DoubleClick is a mobile-first conversational CRM built on top of WhatsApp     Business API to unlock WhatsApp's marketing and sales capabilities. It offers top-notch features, including a central team inbox, bulk broadcasting, and analytics, a bot studio, commerce and cataloging, chatbots, and role-based access. For more details, check out our website: https://doubletick.io/    Activity on InternshalaHiring since April 202455 opportunities posted                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
+          <t>About the internship    Selected intern's day-to-day responsibilities include: 1. Co-create user flows and interfaces for real entertainment products, web experiences, and story-first platforms2. Assist with wireframing, prototyping, and interaction design in Figma (and beyond)3. Help shape gamified UX concepts that mix storytelling, animation, and feedback loops4. Collaborate with storytellers, strategists, devs, and weird creatives to bring new digital formats to life5. Research player psychology, web mechanics, and the fine line between joy and rage-quit6. Bring structure to creative chaos     and chaos to creative structureSkill(s) requiredCreative ThinkingDesign ThinkingTechnical AnalysisTime ManagementUI &amp; UX DesignEarn certifications in these skillsLearn FigmaLearn Rapid PrototypingLearn UI &amp; UX DesignLearn WireframingWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 19th Jul'25 and 23rd Aug'25                                    3. are available for duration of 6 months                                    4. are from Mumbai only                                    5. have relevant skills and interests                    * Women wanting to start/restart their career can also apply.Other requirements                    1. Are graduating in 2025 or 2026 (design school, bootcamp, or self-taught — we care about your mindset, not your certificate)                                    2. Are fluent in UI/UX building tools                                    3. Are excited about interactive storytelling, user behavior, and playful design thinking                PerksCertificate Letter of recommendation Informal dress code Free snacks &amp; beveragesNumber of openings        3                        About OI Communications                        Opinion Incubator (OI) is not a production house. It's a beautifully weaponized idea factory. Born from the mischievous minds behind Red Ice Films, OI marries award-winning storytelling with devilishly precise production craft. We don't chase trends, we seduce them. In a world drowning in content, we create stories that slap, sting, and stay. We don't just make shows; we stage revolutions, irresistible frames at a time.    Activity on InternshalaHiring since July 20252 opportunities posted                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1521,24 +1521,24 @@
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:30</t>
+          <t>2025-07-20 10:41:12</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/customer-support-specialist-internship-in-mumbai-at-apport-software-solutions-private-limited1752826851</t>
+          <t>https://internshala.com/internship/detail/ui-ux-design-internship-in-mumbai-at-oi-communications1752919460</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Business Development (Sales)</t>
+          <t>Industrial And Production Engineering</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>About the internship    Selected intern's day-to-day responsibilities include:1. Identify and engage potential customers through proactive outreach methods,2. Provided tailored information about our products and services to support their decision-making process.3. Address and resolve any objections to achieve sales and secure successful outcomes.4. Oversee and manage sales pipelines and CRM systems to monitor and track leads, and opportunities.Qualifications:1. Bachelor's degree in business administration, marketing, or related field preferred.2. Strong communication and interpersonal skills.3. Ability to engage effectively with diverse audiences.4. Excellent negotiation abilities.5. Stock market knowledge is a plus.Skill(s) requiredClient RelationshipEmail MarketingEnglish Proficiency (Spoken)English Proficiency (Written)SalesEarn certifications in these skillsLearn Email MarketingLearn Business CommunicationLearn Digital MarketingLearn Business AnalyticsWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 18th Jul'25 and 22nd Aug'25                                    3. are available for duration of 3 months                                    4. are from Bangalore only                                    5. have relevant skills and interests                    PerksCertificate Flexible work hours Informal dress code 5 days a week Free snacks &amp; beverages Job offerAdditional informationJob offer: On successful conversion to a permanent employee, the candidate can expect a salary of ₹ 300000 to 360000/year Number of openings        2                        About Trade Brains                Website         Trade Brains is a financial website helping readers learn the art of stock investing, trading, portfolio management, financial planning, money management, and more. At FinGrad (an initiative by Trade Brains), we offer the best online courses, webinars, and resources from various top experts who have real skin in the financial game. FinGrad has been built in the mind to deliver end-to-end financial education at our best standard to our novice investors &amp; traders.    Activity on InternshalaHiring since March 2018545 opportunities posted69 candidates hired                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
+          <t>About the internship    Selected intern's day-to-day responsibilities include: 1. Learn the manufacturing setup2. Work on production management and planning3. Work on research and development activitiesSkill(s) requiredIndustrial automationMechanical &amp; Electrical Product DesignEarn certifications in these skillsLearn CATIALearn Industrial Automation using PLCSolidWorksWho can applyOnly those candidates can apply who:                1. are available for full time (in-office) internship                                    2. can start the internship between 17th Jul'25 and 21st Aug'25                                    3. are available for duration of 3 months                                    4. are from Ujjain only                                    5. have relevant skills and interests                    PerksCertificate Letter of recommendation Informal dress codeNumber of openings        2                        About Rock Engines Private Limited                        Rock Engines Private Limited is a pioneer in the manufacturing of quick oil chamber clean machines and a leading supplier to PSUs, PAN India.     Activity on InternshalaHiring since March 20216 opportunities posted                        Apply now                    Additional Questions×CloseSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            LoginSign up to continue                    Sign up/ Login with Google                                    Sign up with Email                OREmailPasswordFirst NameLast NameSign up                By signing up, you agree to our Terms and Conditions.        Already registered?                            Login</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1556,12 +1556,12 @@
       <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:30</t>
+          <t>2025-07-20 10:41:13</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/business-development-sales-internship-in-bangalore-at-trade-brains1752826094</t>
+          <t>https://internshala.com/internship/detail/industrial-and-production-engineering-internship-in-ujjain-at-rock-engines-private-limited1752747981</t>
         </is>
       </c>
     </row>
@@ -1587,7 +1587,7 @@
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:45</t>
+          <t>2025-07-20 10:41:26</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -1618,7 +1618,7 @@
       <c r="G34" t="inlineStr"/>
       <c r="H34" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:45</t>
+          <t>2025-07-20 10:41:26</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -1649,7 +1649,7 @@
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:45</t>
+          <t>2025-07-20 10:41:26</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -1680,7 +1680,7 @@
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:45</t>
+          <t>2025-07-20 10:41:26</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -1711,7 +1711,7 @@
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:45</t>
+          <t>2025-07-20 10:41:26</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -1742,7 +1742,7 @@
       <c r="G38" t="inlineStr"/>
       <c r="H38" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:45</t>
+          <t>2025-07-20 10:41:26</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -1773,7 +1773,7 @@
       <c r="G39" t="inlineStr"/>
       <c r="H39" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:45</t>
+          <t>2025-07-20 10:41:26</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
@@ -1804,7 +1804,7 @@
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:45</t>
+          <t>2025-07-20 10:41:26</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -1835,7 +1835,7 @@
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:45</t>
+          <t>2025-07-20 10:41:26</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
@@ -1866,7 +1866,7 @@
       <c r="G42" t="inlineStr"/>
       <c r="H42" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:45</t>
+          <t>2025-07-20 10:41:26</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
@@ -1897,7 +1897,7 @@
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:45</t>
+          <t>2025-07-20 10:41:26</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
@@ -1928,7 +1928,7 @@
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:45</t>
+          <t>2025-07-20 10:41:26</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
@@ -1959,7 +1959,7 @@
       <c r="G45" t="inlineStr"/>
       <c r="H45" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:45</t>
+          <t>2025-07-20 10:41:26</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
@@ -1990,7 +1990,7 @@
       <c r="G46" t="inlineStr"/>
       <c r="H46" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:45</t>
+          <t>2025-07-20 10:41:26</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
@@ -2021,7 +2021,7 @@
       <c r="G47" t="inlineStr"/>
       <c r="H47" t="inlineStr">
         <is>
-          <t>2025-07-18 15:28:45</t>
+          <t>2025-07-20 10:41:26</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
@@ -2048,7 +2048,7 @@
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
         <is>
-          <t>2025-07-18 15:29:00</t>
+          <t>2025-07-20 10:41:40</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
@@ -2075,7 +2075,7 @@
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
         <is>
-          <t>2025-07-18 15:29:00</t>
+          <t>2025-07-20 10:41:40</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
@@ -2102,7 +2102,7 @@
       <c r="G50" t="inlineStr"/>
       <c r="H50" t="inlineStr">
         <is>
-          <t>2025-07-18 15:29:00</t>
+          <t>2025-07-20 10:41:40</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
@@ -2129,7 +2129,7 @@
       <c r="G51" t="inlineStr"/>
       <c r="H51" t="inlineStr">
         <is>
-          <t>2025-07-18 15:29:00</t>
+          <t>2025-07-20 10:41:40</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
@@ -2156,7 +2156,7 @@
       <c r="G52" t="inlineStr"/>
       <c r="H52" t="inlineStr">
         <is>
-          <t>2025-07-18 15:29:00</t>
+          <t>2025-07-20 10:41:40</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
@@ -2183,7 +2183,7 @@
       <c r="G53" t="inlineStr"/>
       <c r="H53" t="inlineStr">
         <is>
-          <t>2025-07-18 15:29:01</t>
+          <t>2025-07-20 10:41:40</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
@@ -2210,7 +2210,7 @@
       <c r="G54" t="inlineStr"/>
       <c r="H54" t="inlineStr">
         <is>
-          <t>2025-07-18 15:29:01</t>
+          <t>2025-07-20 10:41:40</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
@@ -2237,7 +2237,7 @@
       <c r="G55" t="inlineStr"/>
       <c r="H55" t="inlineStr">
         <is>
-          <t>2025-07-18 15:29:01</t>
+          <t>2025-07-20 10:41:40</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
@@ -2264,7 +2264,7 @@
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr">
         <is>
-          <t>2025-07-18 15:29:01</t>
+          <t>2025-07-20 10:41:40</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
@@ -2291,7 +2291,7 @@
       <c r="G57" t="inlineStr"/>
       <c r="H57" t="inlineStr">
         <is>
-          <t>2025-07-18 15:29:01</t>
+          <t>2025-07-20 10:41:40</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
@@ -2322,7 +2322,7 @@
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr">
         <is>
-          <t>2025-07-18 15:29:01</t>
+          <t>2025-07-20 10:41:40</t>
         </is>
       </c>
       <c r="I58" t="inlineStr">
@@ -2353,7 +2353,7 @@
       <c r="G59" t="inlineStr"/>
       <c r="H59" t="inlineStr">
         <is>
-          <t>2025-07-18 15:29:01</t>
+          <t>2025-07-20 10:41:40</t>
         </is>
       </c>
       <c r="I59" t="inlineStr">
@@ -2384,7 +2384,7 @@
       <c r="G60" t="inlineStr"/>
       <c r="H60" t="inlineStr">
         <is>
-          <t>2025-07-18 15:29:01</t>
+          <t>2025-07-20 10:41:40</t>
         </is>
       </c>
       <c r="I60" t="inlineStr">
@@ -2415,7 +2415,7 @@
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr">
         <is>
-          <t>2025-07-18 15:29:01</t>
+          <t>2025-07-20 10:41:40</t>
         </is>
       </c>
       <c r="I61" t="inlineStr">
@@ -2446,7 +2446,7 @@
       <c r="G62" t="inlineStr"/>
       <c r="H62" t="inlineStr">
         <is>
-          <t>2025-07-18 15:29:01</t>
+          <t>2025-07-20 10:41:40</t>
         </is>
       </c>
       <c r="I62" t="inlineStr">

</xml_diff>